<commit_message>
Corrigida a formatação de uma tabela em "Estatísticas"
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagoa\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{87022D99-025E-495E-8992-78A7CDF76174}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{09F1DC1A-D623-4882-BA24-7C7C1A338A72}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="4"/>
   </bookViews>
@@ -843,7 +843,7 @@
             <c:numRef>
               <c:f>Estatísticas!$F$14:$F$16</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.80651121760484468</c:v>
@@ -4292,7 +4292,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4542,23 +4542,23 @@
       <c r="A14" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="5">
         <f>SUM('Turma D'!B2:B50)/B6</f>
         <v>0.78787878787878785</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="5">
         <f>SUM('Turma E'!B2:B50)/C6</f>
         <v>0.74193548387096775</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="5">
         <f>SUM('Turma F'!B2:B50)/D6</f>
         <v>0.81818181818181823</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="5">
         <f>SUM('Turma G'!B2:B50)/E6</f>
         <v>0.87804878048780488</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="5">
         <f>AVERAGE(B14:E14)</f>
         <v>0.80651121760484468</v>
       </c>
@@ -4567,23 +4567,23 @@
       <c r="A15" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="5">
         <f>SUM('Turma D'!C2:C50)/B6</f>
         <v>0.63636363636363635</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="5">
         <f>SUM('Turma E'!C2:C50)/C6</f>
         <v>0.58064516129032262</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="5">
         <f>SUM('Turma F'!C2:C50)/D6</f>
         <v>0.72727272727272729</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="5">
         <f>SUM('Turma G'!C2:C50)/E6</f>
         <v>0.68292682926829273</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="5">
         <f>AVERAGE(B15:E15)</f>
         <v>0.65680208854874478</v>
       </c>
@@ -4592,23 +4592,23 @@
       <c r="A16" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="5">
         <f>SUM('Turma D'!D2:D50)/B6</f>
         <v>0.42424242424242425</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="5">
         <f>SUM('Turma E'!D2:D50)/C6</f>
         <v>0.4838709677419355</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="5">
         <f>SUM('Turma F'!D2:D50)/D6</f>
         <v>0.63636363636363635</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="5">
         <f>SUM('Turma G'!D2:D50)/E6</f>
         <v>0.46341463414634149</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="5">
         <f>AVERAGE(B16:E16)</f>
         <v>0.50197291562358437</v>
       </c>

</xml_diff>

<commit_message>
Pequeno ajuste na formação
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagoa\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{09F1DC1A-D623-4882-BA24-7C7C1A338A72}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D645E5E-E059-4BEF-AFDD-CBEABB55FD31}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="4"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Turma D" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,14 @@
     <sheet name="Turma G" sheetId="4" r:id="rId4"/>
     <sheet name="Estatísticas" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -110,7 +117,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -637,9 +644,6 @@
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -655,6 +659,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -846,7 +853,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.80651121760484468</c:v>
+                  <c:v>0.81457573373387693</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.65680208854874478</c:v>
@@ -1918,7 +1925,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1930,6 +1937,7 @@
     <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="8.88671875" style="2"/>
     <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -1989,8 +1997,8 @@
       <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="O2" s="6">
-        <f>(B2*1+C2*2+D2*2)/5</f>
+      <c r="O2" s="5">
+        <f t="shared" ref="O2:O27" si="0">(B2*1+C2*2+D2*2)/5</f>
         <v>1</v>
       </c>
     </row>
@@ -2007,8 +2015,8 @@
       <c r="D3" s="2">
         <v>0</v>
       </c>
-      <c r="O3" s="6">
-        <f>(B3*1+C3*2+D3*2)/5</f>
+      <c r="O3" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -2025,8 +2033,8 @@
       <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="O4" s="6">
-        <f>(B4*1+C4*2+D4*2)/5</f>
+      <c r="O4" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2043,8 +2051,8 @@
       <c r="D5" s="2">
         <v>0</v>
       </c>
-      <c r="O5" s="6">
-        <f>(B5*1+C5*2+D5*2)/5</f>
+      <c r="O5" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -2061,8 +2069,8 @@
       <c r="D6" s="2">
         <v>1</v>
       </c>
-      <c r="O6" s="6">
-        <f>(B6*1+C6*2+D6*2)/5</f>
+      <c r="O6" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2079,8 +2087,8 @@
       <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="O7" s="6">
-        <f>(B7*1+C7*2+D7*2)/5</f>
+      <c r="O7" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2097,8 +2105,8 @@
       <c r="D8" s="2">
         <v>1</v>
       </c>
-      <c r="O8" s="6">
-        <f>(B8*1+C8*2+D8*2)/5</f>
+      <c r="O8" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2115,8 +2123,8 @@
       <c r="D9" s="2">
         <v>0</v>
       </c>
-      <c r="O9" s="6">
-        <f>(B9*1+C9*2+D9*2)/5</f>
+      <c r="O9" s="5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -2133,8 +2141,8 @@
       <c r="D10" s="2">
         <v>1</v>
       </c>
-      <c r="O10" s="6">
-        <f>(B10*1+C10*2+D10*2)/5</f>
+      <c r="O10" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2151,8 +2159,8 @@
       <c r="D11" s="2">
         <v>1</v>
       </c>
-      <c r="O11" s="6">
-        <f>(B11*1+C11*2+D11*2)/5</f>
+      <c r="O11" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2169,8 +2177,8 @@
       <c r="D12" s="2">
         <v>0</v>
       </c>
-      <c r="O12" s="6">
-        <f>(B12*1+C12*2+D12*2)/5</f>
+      <c r="O12" s="5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -2187,8 +2195,8 @@
       <c r="D13" s="2">
         <v>0</v>
       </c>
-      <c r="O13" s="6">
-        <f>(B13*1+C13*2+D13*2)/5</f>
+      <c r="O13" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -2205,8 +2213,8 @@
       <c r="D14" s="2">
         <v>1</v>
       </c>
-      <c r="O14" s="6">
-        <f>(B14*1+C14*2+D14*2)/5</f>
+      <c r="O14" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2223,8 +2231,8 @@
       <c r="D15" s="2">
         <v>1</v>
       </c>
-      <c r="O15" s="6">
-        <f>(B15*1+C15*2+D15*2)/5</f>
+      <c r="O15" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2241,8 +2249,8 @@
       <c r="D16" s="2">
         <v>0</v>
       </c>
-      <c r="O16" s="6">
-        <f>(B16*1+C16*2+D16*2)/5</f>
+      <c r="O16" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -2259,8 +2267,8 @@
       <c r="D17" s="2">
         <v>0</v>
       </c>
-      <c r="O17" s="6">
-        <f>(B17*1+C17*2+D17*2)/5</f>
+      <c r="O17" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -2277,8 +2285,8 @@
       <c r="D18" s="2">
         <v>1</v>
       </c>
-      <c r="O18" s="6">
-        <f>(B18*1+C18*2+D18*2)/5</f>
+      <c r="O18" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2295,8 +2303,8 @@
       <c r="D19" s="2">
         <v>0</v>
       </c>
-      <c r="O19" s="6">
-        <f>(B19*1+C19*2+D19*2)/5</f>
+      <c r="O19" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -2313,8 +2321,8 @@
       <c r="D20" s="2">
         <v>0</v>
       </c>
-      <c r="O20" s="6">
-        <f>(B20*1+C20*2+D20*2)/5</f>
+      <c r="O20" s="5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -2331,8 +2339,8 @@
       <c r="D21" s="2">
         <v>0</v>
       </c>
-      <c r="O21" s="6">
-        <f>(B21*1+C21*2+D21*2)/5</f>
+      <c r="O21" s="5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -2349,8 +2357,8 @@
       <c r="D22" s="2">
         <v>0</v>
       </c>
-      <c r="O22" s="6">
-        <f>(B22*1+C22*2+D22*2)/5</f>
+      <c r="O22" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -2367,8 +2375,8 @@
       <c r="D23" s="2">
         <v>0</v>
       </c>
-      <c r="O23" s="6">
-        <f>(B23*1+C23*2+D23*2)/5</f>
+      <c r="O23" s="5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -2385,8 +2393,8 @@
       <c r="D24" s="2">
         <v>1</v>
       </c>
-      <c r="O24" s="6">
-        <f>(B24*1+C24*2+D24*2)/5</f>
+      <c r="O24" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2403,8 +2411,8 @@
       <c r="D25" s="2">
         <v>1</v>
       </c>
-      <c r="O25" s="6">
-        <f>(B25*1+C25*2+D25*2)/5</f>
+      <c r="O25" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2421,8 +2429,8 @@
       <c r="D26" s="2">
         <v>1</v>
       </c>
-      <c r="O26" s="6">
-        <f>(B26*1+C26*2+D26*2)/5</f>
+      <c r="O26" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2439,8 +2447,8 @@
       <c r="D27" s="2">
         <v>1</v>
       </c>
-      <c r="O27" s="6">
-        <f>(B27*1+C27*2+D27*2)/5</f>
+      <c r="O27" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2464,16 +2472,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:M1"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -2533,8 +2542,8 @@
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="O2" s="6">
-        <f>(B2*1+C2*2+D2*2)/5</f>
+      <c r="O2" s="5">
+        <f t="shared" ref="O2:O27" si="0">(B2*1+C2*2+D2*2)/5</f>
         <v>0.6</v>
       </c>
     </row>
@@ -2551,8 +2560,8 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="O3" s="6">
-        <f>(B3*1+C3*2+D3*2)/5</f>
+      <c r="O3" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2569,8 +2578,8 @@
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="O4" s="6">
-        <f>(B4*1+C4*2+D4*2)/5</f>
+      <c r="O4" s="5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -2587,8 +2596,8 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="O5" s="6">
-        <f>(B5*1+C5*2+D5*2)/5</f>
+      <c r="O5" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -2605,8 +2614,8 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="O6" s="6">
-        <f>(B6*1+C6*2+D6*2)/5</f>
+      <c r="O6" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -2623,8 +2632,8 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="O7" s="6">
-        <f>(B7*1+C7*2+D7*2)/5</f>
+      <c r="O7" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2641,8 +2650,8 @@
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="O8" s="6">
-        <f>(B8*1+C8*2+D8*2)/5</f>
+      <c r="O8" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -2659,8 +2668,8 @@
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="O9" s="6">
-        <f>(B9*1+C9*2+D9*2)/5</f>
+      <c r="O9" s="5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -2677,8 +2686,8 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="O10" s="6">
-        <f>(B10*1+C10*2+D10*2)/5</f>
+      <c r="O10" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2695,8 +2704,8 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="O11" s="6">
-        <f>(B11*1+C11*2+D11*2)/5</f>
+      <c r="O11" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2713,8 +2722,8 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="O12" s="6">
-        <f>(B12*1+C12*2+D12*2)/5</f>
+      <c r="O12" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2731,8 +2740,8 @@
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="O13" s="6">
-        <f>(B13*1+C13*2+D13*2)/5</f>
+      <c r="O13" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -2749,8 +2758,8 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="O14" s="6">
-        <f>(B14*1+C14*2+D14*2)/5</f>
+      <c r="O14" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2767,8 +2776,8 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="O15" s="6">
-        <f>(B15*1+C15*2+D15*2)/5</f>
+      <c r="O15" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2785,8 +2794,8 @@
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="O16" s="6">
-        <f>(B16*1+C16*2+D16*2)/5</f>
+      <c r="O16" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2803,8 +2812,8 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="O17" s="6">
-        <f>(B17*1+C17*2+D17*2)/5</f>
+      <c r="O17" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2821,8 +2830,8 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="O18" s="6">
-        <f>(B18*1+C18*2+D18*2)/5</f>
+      <c r="O18" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2839,8 +2848,8 @@
       <c r="D19">
         <v>1</v>
       </c>
-      <c r="O19" s="6">
-        <f>(B19*1+C19*2+D19*2)/5</f>
+      <c r="O19" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2857,8 +2866,8 @@
       <c r="D20">
         <v>0</v>
       </c>
-      <c r="O20" s="6">
-        <f>(B20*1+C20*2+D20*2)/5</f>
+      <c r="O20" s="5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -2875,8 +2884,8 @@
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="O21" s="6">
-        <f>(B21*1+C21*2+D21*2)/5</f>
+      <c r="O21" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2893,8 +2902,8 @@
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="O22" s="6">
-        <f>(B22*1+C22*2+D22*2)/5</f>
+      <c r="O22" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2911,8 +2920,8 @@
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="O23" s="6">
-        <f>(B23*1+C23*2+D23*2)/5</f>
+      <c r="O23" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2929,28 +2938,34 @@
       <c r="D24">
         <v>0</v>
       </c>
-      <c r="O24" s="6">
-        <f>(B24*1+C24*2+D24*2)/5</f>
+      <c r="O24" s="5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O25" s="6">
-        <f>(B25*1+C25*2+D25*2)/5</f>
-        <v>0</v>
+      <c r="A25">
+        <v>257337</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="O25" s="5">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O26" s="6">
-        <f>(B26*1+C26*2+D26*2)/5</f>
-        <v>0</v>
-      </c>
+      <c r="O26" s="5"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O27" s="6">
-        <f>(B27*1+C27*2+D27*2)/5</f>
-        <v>0</v>
-      </c>
+      <c r="O27" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="O2:O27">
@@ -2970,7 +2985,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3039,8 +3054,8 @@
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="O2" s="6">
-        <f>(B2*1+C2*2+D2*2)/5</f>
+      <c r="O2" s="5">
+        <f t="shared" ref="O2:O30" si="0">(B2*1+C2*2+D2*2)/5</f>
         <v>0.6</v>
       </c>
     </row>
@@ -3057,8 +3072,8 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="O3" s="6">
-        <f>(B3*1+C3*2+D3*2)/5</f>
+      <c r="O3" s="5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -3075,8 +3090,8 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="O4" s="6">
-        <f>(B4*1+C4*2+D4*2)/5</f>
+      <c r="O4" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3093,8 +3108,8 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="O5" s="6">
-        <f>(B5*1+C5*2+D5*2)/5</f>
+      <c r="O5" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -3111,8 +3126,8 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="O6" s="6">
-        <f>(B6*1+C6*2+D6*2)/5</f>
+      <c r="O6" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -3129,8 +3144,8 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="O7" s="6">
-        <f>(B7*1+C7*2+D7*2)/5</f>
+      <c r="O7" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3147,8 +3162,8 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="O8" s="6">
-        <f>(B8*1+C8*2+D8*2)/5</f>
+      <c r="O8" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3165,8 +3180,8 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="O9" s="6">
-        <f>(B9*1+C9*2+D9*2)/5</f>
+      <c r="O9" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3183,8 +3198,8 @@
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="O10" s="6">
-        <f>(B10*1+C10*2+D10*2)/5</f>
+      <c r="O10" s="5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -3201,8 +3216,8 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="O11" s="6">
-        <f>(B11*1+C11*2+D11*2)/5</f>
+      <c r="O11" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3219,8 +3234,8 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="O12" s="6">
-        <f>(B12*1+C12*2+D12*2)/5</f>
+      <c r="O12" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3237,8 +3252,8 @@
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="O13" s="6">
-        <f>(B13*1+C13*2+D13*2)/5</f>
+      <c r="O13" s="5">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3255,8 +3270,8 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="O14" s="6">
-        <f>(B14*1+C14*2+D14*2)/5</f>
+      <c r="O14" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3273,8 +3288,8 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="O15" s="6">
-        <f>(B15*1+C15*2+D15*2)/5</f>
+      <c r="O15" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3291,8 +3306,8 @@
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="O16" s="6">
-        <f>(B16*1+C16*2+D16*2)/5</f>
+      <c r="O16" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3309,8 +3324,8 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="O17" s="6">
-        <f>(B17*1+C17*2+D17*2)/5</f>
+      <c r="O17" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3327,8 +3342,8 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="O18" s="6">
-        <f>(B18*1+C18*2+D18*2)/5</f>
+      <c r="O18" s="5">
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
@@ -3345,8 +3360,8 @@
       <c r="D19">
         <v>1</v>
       </c>
-      <c r="O19" s="6">
-        <f>(B19*1+C19*2+D19*2)/5</f>
+      <c r="O19" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3363,8 +3378,8 @@
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="O20" s="6">
-        <f>(B20*1+C20*2+D20*2)/5</f>
+      <c r="O20" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3381,8 +3396,8 @@
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="O21" s="6">
-        <f>(B21*1+C21*2+D21*2)/5</f>
+      <c r="O21" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3399,8 +3414,8 @@
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="O22" s="6">
-        <f>(B22*1+C22*2+D22*2)/5</f>
+      <c r="O22" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3417,8 +3432,8 @@
       <c r="D23">
         <v>0</v>
       </c>
-      <c r="O23" s="6">
-        <f>(B23*1+C23*2+D23*2)/5</f>
+      <c r="O23" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -3435,8 +3450,8 @@
       <c r="D24">
         <v>1</v>
       </c>
-      <c r="O24" s="6">
-        <f>(B24*1+C24*2+D24*2)/5</f>
+      <c r="O24" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3453,8 +3468,8 @@
       <c r="D25">
         <v>1</v>
       </c>
-      <c r="O25" s="6">
-        <f>(B25*1+C25*2+D25*2)/5</f>
+      <c r="O25" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3471,8 +3486,8 @@
       <c r="D26">
         <v>1</v>
       </c>
-      <c r="O26" s="6">
-        <f>(B26*1+C26*2+D26*2)/5</f>
+      <c r="O26" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3489,8 +3504,8 @@
       <c r="D27">
         <v>1</v>
       </c>
-      <c r="O27" s="6">
-        <f>(B27*1+C27*2+D27*2)/5</f>
+      <c r="O27" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3507,8 +3522,8 @@
       <c r="D28">
         <v>1</v>
       </c>
-      <c r="O28" s="6">
-        <f>(B28*1+C28*2+D28*2)/5</f>
+      <c r="O28" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3525,8 +3540,8 @@
       <c r="D29">
         <v>0</v>
       </c>
-      <c r="O29" s="6">
-        <f>(B29*1+C29*2+D29*2)/5</f>
+      <c r="O29" s="5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -3543,8 +3558,8 @@
       <c r="D30">
         <v>1</v>
       </c>
-      <c r="O30" s="6">
-        <f>(B30*1+C30*2+D30*2)/5</f>
+      <c r="O30" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3566,7 +3581,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3635,8 +3650,8 @@
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="O2" s="6">
-        <f>(B2*1+C2*2+D2*2)/5</f>
+      <c r="O2" s="5">
+        <f t="shared" ref="O2:O37" si="0">(B2*1+C2*2+D2*2)/5</f>
         <v>0.6</v>
       </c>
     </row>
@@ -3653,8 +3668,8 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="O3" s="6">
-        <f>(B3*1+C3*2+D3*2)/5</f>
+      <c r="O3" s="5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -3671,8 +3686,8 @@
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="O4" s="6">
-        <f>(B4*1+C4*2+D4*2)/5</f>
+      <c r="O4" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -3689,8 +3704,8 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="O5" s="6">
-        <f>(B5*1+C5*2+D5*2)/5</f>
+      <c r="O5" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -3707,8 +3722,8 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="O6" s="6">
-        <f>(B6*1+C6*2+D6*2)/5</f>
+      <c r="O6" s="5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -3725,8 +3740,8 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="O7" s="6">
-        <f>(B7*1+C7*2+D7*2)/5</f>
+      <c r="O7" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3743,8 +3758,8 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="O8" s="6">
-        <f>(B8*1+C8*2+D8*2)/5</f>
+      <c r="O8" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3761,8 +3776,8 @@
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="O9" s="6">
-        <f>(B9*1+C9*2+D9*2)/5</f>
+      <c r="O9" s="5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -3779,8 +3794,8 @@
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="O10" s="6">
-        <f>(B10*1+C10*2+D10*2)/5</f>
+      <c r="O10" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -3797,8 +3812,8 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="O11" s="6">
-        <f>(B11*1+C11*2+D11*2)/5</f>
+      <c r="O11" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3815,8 +3830,8 @@
       <c r="D12">
         <v>0</v>
       </c>
-      <c r="O12" s="6">
-        <f>(B12*1+C12*2+D12*2)/5</f>
+      <c r="O12" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -3833,8 +3848,8 @@
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="O13" s="6">
-        <f>(B13*1+C13*2+D13*2)/5</f>
+      <c r="O13" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -3851,8 +3866,8 @@
       <c r="D14">
         <v>0</v>
       </c>
-      <c r="O14" s="6">
-        <f>(B14*1+C14*2+D14*2)/5</f>
+      <c r="O14" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -3869,8 +3884,8 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="O15" s="6">
-        <f>(B15*1+C15*2+D15*2)/5</f>
+      <c r="O15" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3887,8 +3902,8 @@
       <c r="D16">
         <v>0</v>
       </c>
-      <c r="O16" s="6">
-        <f>(B16*1+C16*2+D16*2)/5</f>
+      <c r="O16" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -3905,8 +3920,8 @@
       <c r="D17">
         <v>0</v>
       </c>
-      <c r="O17" s="6">
-        <f>(B17*1+C17*2+D17*2)/5</f>
+      <c r="O17" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -3923,8 +3938,8 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="O18" s="6">
-        <f>(B18*1+C18*2+D18*2)/5</f>
+      <c r="O18" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3941,8 +3956,8 @@
       <c r="D19">
         <v>1</v>
       </c>
-      <c r="O19" s="6">
-        <f>(B19*1+C19*2+D19*2)/5</f>
+      <c r="O19" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3959,8 +3974,8 @@
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="O20" s="6">
-        <f>(B20*1+C20*2+D20*2)/5</f>
+      <c r="O20" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3977,8 +3992,8 @@
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="O21" s="6">
-        <f>(B21*1+C21*2+D21*2)/5</f>
+      <c r="O21" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3995,8 +4010,8 @@
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="O22" s="6">
-        <f>(B22*1+C22*2+D22*2)/5</f>
+      <c r="O22" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4013,8 +4028,8 @@
       <c r="D23">
         <v>1</v>
       </c>
-      <c r="O23" s="6">
-        <f>(B23*1+C23*2+D23*2)/5</f>
+      <c r="O23" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4031,8 +4046,8 @@
       <c r="D24">
         <v>0</v>
       </c>
-      <c r="O24" s="6">
-        <f>(B24*1+C24*2+D24*2)/5</f>
+      <c r="O24" s="5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -4049,8 +4064,8 @@
       <c r="D25">
         <v>1</v>
       </c>
-      <c r="O25" s="6">
-        <f>(B25*1+C25*2+D25*2)/5</f>
+      <c r="O25" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4067,8 +4082,8 @@
       <c r="D26">
         <v>0</v>
       </c>
-      <c r="O26" s="6">
-        <f>(B26*1+C26*2+D26*2)/5</f>
+      <c r="O26" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -4085,8 +4100,8 @@
       <c r="D27">
         <v>1</v>
       </c>
-      <c r="O27" s="6">
-        <f>(B27*1+C27*2+D27*2)/5</f>
+      <c r="O27" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4103,8 +4118,8 @@
       <c r="D28">
         <v>1</v>
       </c>
-      <c r="O28" s="6">
-        <f>(B28*1+C28*2+D28*2)/5</f>
+      <c r="O28" s="5">
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -4121,8 +4136,8 @@
       <c r="D29">
         <v>0</v>
       </c>
-      <c r="O29" s="6">
-        <f>(B29*1+C29*2+D29*2)/5</f>
+      <c r="O29" s="5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -4139,8 +4154,8 @@
       <c r="D30">
         <v>0</v>
       </c>
-      <c r="O30" s="6">
-        <f>(B30*1+C30*2+D30*2)/5</f>
+      <c r="O30" s="5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -4157,8 +4172,8 @@
       <c r="D31">
         <v>1</v>
       </c>
-      <c r="O31" s="6">
-        <f>(B31*1+C31*2+D31*2)/5</f>
+      <c r="O31" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4175,8 +4190,8 @@
       <c r="D32">
         <v>1</v>
       </c>
-      <c r="O32" s="6">
-        <f>(B32*1+C32*2+D32*2)/5</f>
+      <c r="O32" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4193,8 +4208,8 @@
       <c r="D33">
         <v>1</v>
       </c>
-      <c r="O33" s="6">
-        <f>(B33*1+C33*2+D33*2)/5</f>
+      <c r="O33" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4211,8 +4226,8 @@
       <c r="D34">
         <v>1</v>
       </c>
-      <c r="O34" s="6">
-        <f>(B34*1+C34*2+D34*2)/5</f>
+      <c r="O34" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4229,8 +4244,8 @@
       <c r="D35">
         <v>1</v>
       </c>
-      <c r="O35" s="6">
-        <f>(B35*1+C35*2+D35*2)/5</f>
+      <c r="O35" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4247,8 +4262,8 @@
       <c r="D36">
         <v>1</v>
       </c>
-      <c r="O36" s="6">
-        <f>(B36*1+C36*2+D36*2)/5</f>
+      <c r="O36" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4265,8 +4280,8 @@
       <c r="D37">
         <v>0</v>
       </c>
-      <c r="O37" s="6">
-        <f>(B37*1+C37*2+D37*2)/5</f>
+      <c r="O37" s="5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -4288,11 +4303,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4301,7 +4316,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -4342,7 +4357,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
+      <c r="A2" s="11"/>
       <c r="B2" s="2">
         <v>1</v>
       </c>
@@ -4398,7 +4413,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B6">
@@ -4419,110 +4434,110 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B7">
-        <f>COUNTA('Turma D'!A2:A45)</f>
+        <f>COUNTA('Turma D'!A2:A50)</f>
         <v>26</v>
       </c>
       <c r="C7">
-        <f>COUNTA('Turma E'!A2:A45)</f>
-        <v>23</v>
+        <f>COUNTA('Turma E'!A2:A50)</f>
+        <v>24</v>
       </c>
       <c r="D7">
-        <f>COUNTA('Turma F'!A2:A45)</f>
+        <f>COUNTA('Turma F'!A2:A50)</f>
         <v>29</v>
       </c>
       <c r="E7">
-        <f>COUNTA('Turma G'!A2:A45)</f>
+        <f>COUNTA('Turma G'!A2:A50)</f>
         <v>36</v>
       </c>
       <c r="F7">
         <f>SUM(B7:E7)</f>
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <f>(B7/B6)</f>
         <v>0.78787878787878785</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <f t="shared" ref="C8:F8" si="0">(C7/C6)</f>
-        <v>0.74193548387096775</v>
-      </c>
-      <c r="D8" s="5">
+        <v>0.77419354838709675</v>
+      </c>
+      <c r="D8" s="4">
         <f t="shared" si="0"/>
         <v>0.87878787878787878</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <f t="shared" si="0"/>
         <v>0.87804878048780488</v>
       </c>
-      <c r="F8" s="5">
-        <f t="shared" si="0"/>
-        <v>0.82608695652173914</v>
+      <c r="F8" s="4">
+        <f t="shared" si="0"/>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <f>SUM('Turma D'!O2:O50)/B6</f>
         <v>0.58181818181818168</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <f>SUM('Turma E'!O2:O50)/C6</f>
-        <v>0.5741935483870968</v>
-      </c>
-      <c r="D9" s="5">
+        <v>0.58064516129032262</v>
+      </c>
+      <c r="D9" s="4">
         <f>SUM('Turma F'!O2:O50)/D6</f>
         <v>0.70909090909090911</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <f>SUM('Turma G'!O2:O50)/E6</f>
         <v>0.63414634146341464</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <f>AVERAGE(B9:E9)</f>
-        <v>0.62481224518990053</v>
+        <v>0.62642514841570707</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <f>SUM('Turma D'!O2:O50)/B7</f>
         <v>0.73846153846153828</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <f>SUM('Turma E'!O2:O50)/C7</f>
-        <v>0.77391304347826095</v>
-      </c>
-      <c r="D10" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="D10" s="4">
         <f>SUM('Turma F'!O2:O50)/D7</f>
         <v>0.80689655172413799</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <f>SUM('Turma G'!O2:O50)/E7</f>
         <v>0.72222222222222221</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <f>AVERAGE(B10:E10)</f>
-        <v>0.76037333897153991</v>
+        <v>0.75439507810197459</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -4539,128 +4554,128 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="5">
+      <c r="A14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="4">
         <f>SUM('Turma D'!B2:B50)/B6</f>
         <v>0.78787878787878785</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <f>SUM('Turma E'!B2:B50)/C6</f>
-        <v>0.74193548387096775</v>
-      </c>
-      <c r="D14" s="5">
+        <v>0.77419354838709675</v>
+      </c>
+      <c r="D14" s="4">
         <f>SUM('Turma F'!B2:B50)/D6</f>
         <v>0.81818181818181823</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <f>SUM('Turma G'!B2:B50)/E6</f>
         <v>0.87804878048780488</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <f>AVERAGE(B14:E14)</f>
-        <v>0.80651121760484468</v>
+        <v>0.81457573373387693</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <f>SUM('Turma D'!C2:C50)/B6</f>
         <v>0.63636363636363635</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <f>SUM('Turma E'!C2:C50)/C6</f>
         <v>0.58064516129032262</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <f>SUM('Turma F'!C2:C50)/D6</f>
         <v>0.72727272727272729</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <f>SUM('Turma G'!C2:C50)/E6</f>
         <v>0.68292682926829273</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <f>AVERAGE(B15:E15)</f>
         <v>0.65680208854874478</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <f>SUM('Turma D'!D2:D50)/B6</f>
         <v>0.42424242424242425</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <f>SUM('Turma E'!D2:D50)/C6</f>
         <v>0.4838709677419355</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <f>SUM('Turma F'!D2:D50)/D6</f>
         <v>0.63636363636363635</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <f>SUM('Turma G'!D2:D50)/E6</f>
         <v>0.46341463414634149</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="4">
         <f>AVERAGE(B16:E16)</f>
         <v>0.50197291562358437</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="9"/>
+      <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
+      <c r="A26" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Adicionado notas do Lab 04
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagoa\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D645E5E-E059-4BEF-AFDD-CBEABB55FD31}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A45E983-404E-4D23-B710-40375FCED30C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="27">
   <si>
     <t>RA</t>
   </si>
@@ -447,7 +447,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -563,15 +563,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="0"/>
       </left>
@@ -654,15 +645,17 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -831,9 +824,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Estatísticas!$A$14:$A$16</c:f>
+              <c:f>Estatísticas!$A$14:$A$17</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Lab 01</c:v>
                 </c:pt>
@@ -843,15 +836,18 @@
                 <c:pt idx="2">
                   <c:v>Lab 03</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>Lab 04</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Estatísticas!$F$14:$F$16</c:f>
+              <c:f>Estatísticas!$F$14:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.81457573373387693</c:v>
                 </c:pt>
@@ -860,6 +856,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.50197291562358437</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.49656080871659158</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1926,10 +1925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1997,8 +1996,11 @@
       <c r="D2" s="2">
         <v>1</v>
       </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
       <c r="O2" s="5">
-        <f t="shared" ref="O2:O27" si="0">(B2*1+C2*2+D2*2)/5</f>
+        <f>(B2*1+C2*2+D2*2+E2*3)/8</f>
         <v>1</v>
       </c>
     </row>
@@ -2015,9 +2017,12 @@
       <c r="D3" s="2">
         <v>0</v>
       </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
       <c r="O3" s="5">
-        <f t="shared" si="0"/>
-        <v>0.6</v>
+        <f t="shared" ref="O3:O29" si="0">(B3*1+C3*2+D3*2+E3*3)/8</f>
+        <v>0.375</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -2033,6 +2038,9 @@
       <c r="D4" s="2">
         <v>1</v>
       </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
       <c r="O4" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2051,9 +2059,12 @@
       <c r="D5" s="2">
         <v>0</v>
       </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
       <c r="O5" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -2069,6 +2080,9 @@
       <c r="D6" s="2">
         <v>1</v>
       </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
       <c r="O6" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2087,9 +2101,12 @@
       <c r="D7" s="2">
         <v>1</v>
       </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
       <c r="O7" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -2105,6 +2122,9 @@
       <c r="D8" s="2">
         <v>1</v>
       </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
       <c r="O8" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2123,9 +2143,12 @@
       <c r="D9" s="2">
         <v>0</v>
       </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
       <c r="O9" s="5">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -2141,6 +2164,9 @@
       <c r="D10" s="2">
         <v>1</v>
       </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
       <c r="O10" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2159,9 +2185,12 @@
       <c r="D11" s="2">
         <v>1</v>
       </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
       <c r="O11" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -2177,9 +2206,12 @@
       <c r="D12" s="2">
         <v>0</v>
       </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
       <c r="O12" s="5">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -2195,9 +2227,12 @@
       <c r="D13" s="2">
         <v>0</v>
       </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
       <c r="O13" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -2213,6 +2248,9 @@
       <c r="D14" s="2">
         <v>1</v>
       </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
       <c r="O14" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2220,25 +2258,28 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>224176</v>
+        <v>221215</v>
       </c>
       <c r="B15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
       </c>
       <c r="O15" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>225295</v>
+        <v>224176</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
@@ -2247,16 +2288,19 @@
         <v>1</v>
       </c>
       <c r="D16" s="2">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
       </c>
       <c r="O16" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>232239</v>
+        <v>225295</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
@@ -2267,14 +2311,17 @@
       <c r="D17" s="2">
         <v>0</v>
       </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
       <c r="O17" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>233901</v>
+        <v>232239</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
@@ -2283,16 +2330,19 @@
         <v>1</v>
       </c>
       <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18">
         <v>1</v>
       </c>
       <c r="O18" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>235914</v>
+        <v>233901</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>
@@ -2301,19 +2351,22 @@
         <v>1</v>
       </c>
       <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19">
         <v>0</v>
       </c>
       <c r="O19" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>235997</v>
+        <v>233901</v>
       </c>
       <c r="B20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="2">
         <v>0</v>
@@ -2321,50 +2374,59 @@
       <c r="D20" s="2">
         <v>0</v>
       </c>
+      <c r="E20" s="11">
+        <v>1</v>
+      </c>
       <c r="O20" s="5">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>237668</v>
+        <v>235914</v>
       </c>
       <c r="B21" s="2">
         <v>1</v>
       </c>
       <c r="C21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2">
         <v>0</v>
       </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
       <c r="O21" s="5">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>237870</v>
+        <v>235997</v>
       </c>
       <c r="B22" s="2">
         <v>1</v>
       </c>
       <c r="C22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="2">
         <v>0</v>
       </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
       <c r="O22" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>238916</v>
+        <v>237668</v>
       </c>
       <c r="B23" s="2">
         <v>1</v>
@@ -2375,14 +2437,17 @@
       <c r="D23" s="2">
         <v>0</v>
       </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
       <c r="O23" s="5">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>240195</v>
+        <v>237870</v>
       </c>
       <c r="B24" s="2">
         <v>1</v>
@@ -2391,34 +2456,40 @@
         <v>1</v>
       </c>
       <c r="D24" s="2">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
       </c>
       <c r="O24" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>240352</v>
+        <v>238916</v>
       </c>
       <c r="B25" s="2">
         <v>1</v>
       </c>
       <c r="C25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25">
         <v>1</v>
       </c>
       <c r="O25" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>244540</v>
+        <v>240195</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
@@ -2427,6 +2498,9 @@
         <v>1</v>
       </c>
       <c r="D26" s="2">
+        <v>1</v>
+      </c>
+      <c r="E26">
         <v>1</v>
       </c>
       <c r="O26" s="5">
@@ -2436,25 +2510,70 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27">
+        <v>240352</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="O27" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>244540</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="O28" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29">
         <v>261031</v>
       </c>
-      <c r="B27" s="2">
-        <v>1</v>
-      </c>
-      <c r="C27" s="2">
-        <v>1</v>
-      </c>
-      <c r="D27" s="2">
-        <v>1</v>
-      </c>
-      <c r="O27" s="5">
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="O29" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="O2:O27">
+  <conditionalFormatting sqref="O2:O29">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2476,7 +2595,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="O2" sqref="O2:O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2542,9 +2661,12 @@
       <c r="D2">
         <v>0</v>
       </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
       <c r="O2" s="5">
-        <f t="shared" ref="O2:O27" si="0">(B2*1+C2*2+D2*2)/5</f>
-        <v>0.6</v>
+        <f>(B2*1+C2*2+D2*2+E2*3)/8</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -2560,9 +2682,12 @@
       <c r="D3">
         <v>1</v>
       </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
       <c r="O3" s="5">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" ref="O3:O25" si="0">(B3*1+C3*2+D3*2+E3*3)/8</f>
+        <v>0.625</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -2578,9 +2703,12 @@
       <c r="D4">
         <v>0</v>
       </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
       <c r="O4" s="5">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -2596,9 +2724,12 @@
       <c r="D5">
         <v>1</v>
       </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
       <c r="O5" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -2614,9 +2745,12 @@
       <c r="D6">
         <v>0</v>
       </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
       <c r="O6" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -2632,6 +2766,9 @@
       <c r="D7">
         <v>1</v>
       </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
       <c r="O7" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2650,9 +2787,12 @@
       <c r="D8">
         <v>0</v>
       </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
       <c r="O8" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -2668,9 +2808,12 @@
       <c r="D9">
         <v>0</v>
       </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
       <c r="O9" s="5">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -2686,6 +2829,9 @@
       <c r="D10">
         <v>1</v>
       </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
       <c r="O10" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2704,9 +2850,12 @@
       <c r="D11">
         <v>1</v>
       </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
       <c r="O11" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -2722,6 +2871,9 @@
       <c r="D12">
         <v>1</v>
       </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
       <c r="O12" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2740,9 +2892,12 @@
       <c r="D13">
         <v>0</v>
       </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
       <c r="O13" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -2758,6 +2913,9 @@
       <c r="D14">
         <v>1</v>
       </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
       <c r="O14" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2776,6 +2934,9 @@
       <c r="D15">
         <v>1</v>
       </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
       <c r="O15" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2794,6 +2955,9 @@
       <c r="D16">
         <v>1</v>
       </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
       <c r="O16" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2812,9 +2976,12 @@
       <c r="D17">
         <v>1</v>
       </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
       <c r="O17" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -2830,6 +2997,9 @@
       <c r="D18">
         <v>1</v>
       </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
       <c r="O18" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2848,6 +3018,9 @@
       <c r="D19">
         <v>1</v>
       </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
       <c r="O19" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2866,9 +3039,12 @@
       <c r="D20">
         <v>0</v>
       </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
       <c r="O20" s="5">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -2884,6 +3060,9 @@
       <c r="D21">
         <v>1</v>
       </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
       <c r="O21" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2902,9 +3081,12 @@
       <c r="D22">
         <v>1</v>
       </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
       <c r="O22" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -2920,6 +3102,9 @@
       <c r="D23">
         <v>1</v>
       </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
       <c r="O23" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2938,9 +3123,12 @@
       <c r="D24">
         <v>0</v>
       </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
       <c r="O24" s="5">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -2956,9 +3144,12 @@
       <c r="D25">
         <v>0</v>
       </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
       <c r="O25" s="5">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -2989,7 +3180,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="O2" sqref="O2:O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3054,9 +3245,12 @@
       <c r="D2">
         <v>0</v>
       </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
       <c r="O2" s="5">
-        <f t="shared" ref="O2:O30" si="0">(B2*1+C2*2+D2*2)/5</f>
-        <v>0.6</v>
+        <f>(B2*1+C2*2+D2*2+E2*3)/8</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -3072,9 +3266,12 @@
       <c r="D3">
         <v>0</v>
       </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
       <c r="O3" s="5">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
+        <f t="shared" ref="O3:O30" si="0">(B3*1+C3*2+D3*2+E3*3)/8</f>
+        <v>0.125</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -3090,9 +3287,12 @@
       <c r="D4">
         <v>1</v>
       </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
       <c r="O4" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -3108,9 +3308,12 @@
       <c r="D5">
         <v>0</v>
       </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
       <c r="O5" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -3126,9 +3329,12 @@
       <c r="D6">
         <v>0</v>
       </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
       <c r="O6" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -3144,6 +3350,9 @@
       <c r="D7">
         <v>1</v>
       </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
       <c r="O7" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3162,6 +3371,9 @@
       <c r="D8">
         <v>1</v>
       </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
       <c r="O8" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3180,9 +3392,12 @@
       <c r="D9">
         <v>1</v>
       </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
       <c r="O9" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -3198,9 +3413,12 @@
       <c r="D10">
         <v>0</v>
       </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
       <c r="O10" s="5">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -3216,6 +3434,9 @@
       <c r="D11">
         <v>1</v>
       </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
       <c r="O11" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3234,6 +3455,9 @@
       <c r="D12">
         <v>1</v>
       </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
       <c r="O12" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3252,6 +3476,9 @@
       <c r="D13">
         <v>0</v>
       </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
       <c r="O13" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3270,6 +3497,9 @@
       <c r="D14">
         <v>1</v>
       </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
       <c r="O14" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3288,6 +3518,9 @@
       <c r="D15">
         <v>1</v>
       </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
       <c r="O15" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3306,6 +3539,9 @@
       <c r="D16">
         <v>1</v>
       </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
       <c r="O16" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3324,6 +3560,9 @@
       <c r="D17">
         <v>1</v>
       </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
       <c r="O17" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3342,9 +3581,12 @@
       <c r="D18">
         <v>1</v>
       </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
       <c r="O18" s="5">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -3360,9 +3602,12 @@
       <c r="D19">
         <v>1</v>
       </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
       <c r="O19" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -3378,6 +3623,9 @@
       <c r="D20">
         <v>1</v>
       </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
       <c r="O20" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3396,6 +3644,9 @@
       <c r="D21">
         <v>1</v>
       </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
       <c r="O21" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3414,6 +3665,9 @@
       <c r="D22">
         <v>1</v>
       </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
       <c r="O22" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3432,9 +3686,12 @@
       <c r="D23">
         <v>0</v>
       </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
       <c r="O23" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -3450,6 +3707,9 @@
       <c r="D24">
         <v>1</v>
       </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
       <c r="O24" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3468,6 +3728,9 @@
       <c r="D25">
         <v>1</v>
       </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
       <c r="O25" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3486,6 +3749,9 @@
       <c r="D26">
         <v>1</v>
       </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
       <c r="O26" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3504,6 +3770,9 @@
       <c r="D27">
         <v>1</v>
       </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
       <c r="O27" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3522,6 +3791,9 @@
       <c r="D28">
         <v>1</v>
       </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
       <c r="O28" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3540,9 +3812,12 @@
       <c r="D29">
         <v>0</v>
       </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
       <c r="O29" s="5">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -3556,6 +3831,9 @@
         <v>1</v>
       </c>
       <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
         <v>1</v>
       </c>
       <c r="O30" s="5">
@@ -3585,7 +3863,7 @@
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3650,9 +3928,12 @@
       <c r="D2">
         <v>0</v>
       </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
       <c r="O2" s="5">
-        <f t="shared" ref="O2:O37" si="0">(B2*1+C2*2+D2*2)/5</f>
-        <v>0.6</v>
+        <f>(B2*1+C2*2+D2*2+E2*3)/8</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -3668,9 +3949,12 @@
       <c r="D3">
         <v>0</v>
       </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
       <c r="O3" s="5">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
+        <f t="shared" ref="O3:O37" si="0">(B3*1+C3*2+D3*2+E3*3)/8</f>
+        <v>0.125</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -3686,9 +3970,12 @@
       <c r="D4">
         <v>0</v>
       </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
       <c r="O4" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -3704,9 +3991,12 @@
       <c r="D5">
         <v>0</v>
       </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
       <c r="O5" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -3722,9 +4012,12 @@
       <c r="D6">
         <v>0</v>
       </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
       <c r="O6" s="5">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -3740,6 +4033,9 @@
       <c r="D7">
         <v>1</v>
       </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
       <c r="O7" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3758,6 +4054,9 @@
       <c r="D8">
         <v>1</v>
       </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
       <c r="O8" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3776,9 +4075,12 @@
       <c r="D9">
         <v>0</v>
       </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
       <c r="O9" s="5">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -3794,9 +4096,12 @@
       <c r="D10">
         <v>0</v>
       </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
       <c r="O10" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -3812,6 +4117,9 @@
       <c r="D11">
         <v>1</v>
       </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
       <c r="O11" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3830,9 +4138,12 @@
       <c r="D12">
         <v>0</v>
       </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
       <c r="O12" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -3848,9 +4159,12 @@
       <c r="D13">
         <v>0</v>
       </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
       <c r="O13" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -3866,9 +4180,12 @@
       <c r="D14">
         <v>0</v>
       </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
       <c r="O14" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -3884,6 +4201,9 @@
       <c r="D15">
         <v>1</v>
       </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
       <c r="O15" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3902,9 +4222,12 @@
       <c r="D16">
         <v>0</v>
       </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
       <c r="O16" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -3920,9 +4243,12 @@
       <c r="D17">
         <v>0</v>
       </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
       <c r="O17" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -3938,6 +4264,9 @@
       <c r="D18">
         <v>1</v>
       </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
       <c r="O18" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3956,6 +4285,9 @@
       <c r="D19">
         <v>1</v>
       </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
       <c r="O19" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3974,6 +4306,9 @@
       <c r="D20">
         <v>1</v>
       </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
       <c r="O20" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3992,6 +4327,9 @@
       <c r="D21">
         <v>1</v>
       </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
       <c r="O21" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4010,6 +4348,9 @@
       <c r="D22">
         <v>1</v>
       </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
       <c r="O22" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4028,6 +4369,9 @@
       <c r="D23">
         <v>1</v>
       </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
       <c r="O23" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4046,9 +4390,12 @@
       <c r="D24">
         <v>0</v>
       </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
       <c r="O24" s="5">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -4064,6 +4411,9 @@
       <c r="D25">
         <v>1</v>
       </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
       <c r="O25" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4082,9 +4432,12 @@
       <c r="D26">
         <v>0</v>
       </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
       <c r="O26" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -4100,6 +4453,9 @@
       <c r="D27">
         <v>1</v>
       </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
       <c r="O27" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4118,9 +4474,12 @@
       <c r="D28">
         <v>1</v>
       </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
       <c r="O28" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -4136,9 +4495,12 @@
       <c r="D29">
         <v>0</v>
       </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
       <c r="O29" s="5">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -4154,9 +4516,12 @@
       <c r="D30">
         <v>0</v>
       </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
       <c r="O30" s="5">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -4172,9 +4537,12 @@
       <c r="D31">
         <v>1</v>
       </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
       <c r="O31" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
@@ -4190,9 +4558,12 @@
       <c r="D32">
         <v>1</v>
       </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
       <c r="O32" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
@@ -4208,9 +4579,12 @@
       <c r="D33">
         <v>1</v>
       </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
       <c r="O33" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
@@ -4226,6 +4600,9 @@
       <c r="D34">
         <v>1</v>
       </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
       <c r="O34" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4244,6 +4621,9 @@
       <c r="D35">
         <v>1</v>
       </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
       <c r="O35" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4262,6 +4642,9 @@
       <c r="D36">
         <v>1</v>
       </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
       <c r="O36" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4280,9 +4663,12 @@
       <c r="D37">
         <v>0</v>
       </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
       <c r="O37" s="5">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
     </row>
   </sheetData>
@@ -4307,16 +4693,19 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -4357,7 +4746,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
+      <c r="A2" s="10"/>
       <c r="B2" s="2">
         <v>1</v>
       </c>
@@ -4370,14 +4759,14 @@
       <c r="E2" s="2">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>23</v>
+      <c r="F2" s="2">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <v>3</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>23</v>
@@ -4439,7 +4828,7 @@
       </c>
       <c r="B7">
         <f>COUNTA('Turma D'!A2:A50)</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C7">
         <f>COUNTA('Turma E'!A2:A50)</f>
@@ -4455,7 +4844,7 @@
       </c>
       <c r="F7">
         <f>SUM(B7:E7)</f>
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -4464,10 +4853,10 @@
       </c>
       <c r="B8" s="4">
         <f>(B7/B6)</f>
-        <v>0.78787878787878785</v>
+        <v>0.84848484848484851</v>
       </c>
       <c r="C8" s="4">
-        <f t="shared" ref="C8:F8" si="0">(C7/C6)</f>
+        <f t="shared" ref="C8:F9" si="0">(C7/C6)</f>
         <v>0.77419354838709675</v>
       </c>
       <c r="D8" s="4">
@@ -4480,7 +4869,7 @@
       </c>
       <c r="F8" s="4">
         <f t="shared" si="0"/>
-        <v>0.83333333333333337</v>
+        <v>0.84782608695652173</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -4489,23 +4878,23 @@
       </c>
       <c r="B9" s="4">
         <f>SUM('Turma D'!O2:O50)/B6</f>
-        <v>0.58181818181818168</v>
+        <v>0.53409090909090906</v>
       </c>
       <c r="C9" s="4">
         <f>SUM('Turma E'!O2:O50)/C6</f>
-        <v>0.58064516129032262</v>
+        <v>0.52016129032258063</v>
       </c>
       <c r="D9" s="4">
         <f>SUM('Turma F'!O2:O50)/D6</f>
-        <v>0.70909090909090911</v>
+        <v>0.65909090909090906</v>
       </c>
       <c r="E9" s="4">
         <f>SUM('Turma G'!O2:O50)/E6</f>
-        <v>0.63414634146341464</v>
+        <v>0.59756097560975607</v>
       </c>
       <c r="F9" s="4">
-        <f>AVERAGE(B9:E9)</f>
-        <v>0.62642514841570707</v>
+        <f t="shared" si="0"/>
+        <v>7.246376811594203E-3</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -4514,30 +4903,30 @@
       </c>
       <c r="B10" s="4">
         <f>SUM('Turma D'!O2:O50)/B7</f>
-        <v>0.73846153846153828</v>
+        <v>0.6294642857142857</v>
       </c>
       <c r="C10" s="4">
         <f>SUM('Turma E'!O2:O50)/C7</f>
-        <v>0.75</v>
+        <v>0.671875</v>
       </c>
       <c r="D10" s="4">
         <f>SUM('Turma F'!O2:O50)/D7</f>
-        <v>0.80689655172413799</v>
+        <v>0.75</v>
       </c>
       <c r="E10" s="4">
         <f>SUM('Turma G'!O2:O50)/E7</f>
-        <v>0.72222222222222221</v>
+        <v>0.68055555555555558</v>
       </c>
       <c r="F10" s="4">
         <f>AVERAGE(B10:E10)</f>
-        <v>0.75439507810197459</v>
+        <v>0.68297371031746024</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -4632,6 +5021,26 @@
       <c r="A17" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="B17" s="4">
+        <f>SUM('Turma D'!E2:E50)/B6</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="C17" s="4">
+        <f>SUM('Turma E'!E2:E50)/C6</f>
+        <v>0.41935483870967744</v>
+      </c>
+      <c r="D17" s="4">
+        <f>SUM('Turma F'!E2:E50)/D6</f>
+        <v>0.5757575757575758</v>
+      </c>
+      <c r="E17" s="4">
+        <f>SUM('Turma G'!E2:E50)/E6</f>
+        <v>0.53658536585365857</v>
+      </c>
+      <c r="F17" s="4">
+        <f>AVERAGE(B17:E17)</f>
+        <v>0.49656080871659158</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
@@ -4642,7 +5051,6 @@
       <c r="A19" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">

</xml_diff>

<commit_message>
Corrigido uma fórmula errada no sumário das notas
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagoa\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A45E983-404E-4D23-B710-40375FCED30C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC453645-1635-418D-A7C8-82DC5E5D287D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -651,11 +651,11 @@
     <xf numFmtId="0" fontId="13" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2374,7 +2374,7 @@
       <c r="D20" s="2">
         <v>0</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="10">
         <v>1</v>
       </c>
       <c r="O20" s="5">
@@ -4693,7 +4693,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4705,7 +4705,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -4746,7 +4746,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
+      <c r="A2" s="11"/>
       <c r="B2" s="2">
         <v>1</v>
       </c>
@@ -4893,8 +4893,8 @@
         <v>0.59756097560975607</v>
       </c>
       <c r="F9" s="4">
-        <f t="shared" si="0"/>
-        <v>7.246376811594203E-3</v>
+        <f>AVERAGE(B9:E9)</f>
+        <v>0.57772602102853876</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Erro de digitação em uma nota da Turma D
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagoa\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagoa\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC453645-1635-418D-A7C8-82DC5E5D287D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73F6EE4-F177-4A1E-8037-B1DC196B2C85}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Turma D" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Turma G" sheetId="4" r:id="rId4"/>
     <sheet name="Estatísticas" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -858,7 +858,7 @@
                   <c:v>0.50197291562358437</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.49656080871659158</c:v>
+                  <c:v>0.50413656629234915</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1927,8 +1927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2354,11 +2354,11 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O19" s="5">
         <f t="shared" si="0"/>
-        <v>0.625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -4692,7 +4692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -4856,7 +4856,7 @@
         <v>0.84848484848484851</v>
       </c>
       <c r="C8" s="4">
-        <f t="shared" ref="C8:F9" si="0">(C7/C6)</f>
+        <f t="shared" ref="C8:F8" si="0">(C7/C6)</f>
         <v>0.77419354838709675</v>
       </c>
       <c r="D8" s="4">
@@ -4878,7 +4878,7 @@
       </c>
       <c r="B9" s="4">
         <f>SUM('Turma D'!O2:O50)/B6</f>
-        <v>0.53409090909090906</v>
+        <v>0.54545454545454541</v>
       </c>
       <c r="C9" s="4">
         <f>SUM('Turma E'!O2:O50)/C6</f>
@@ -4894,7 +4894,7 @@
       </c>
       <c r="F9" s="4">
         <f>AVERAGE(B9:E9)</f>
-        <v>0.57772602102853876</v>
+        <v>0.58056693011944782</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -4903,7 +4903,7 @@
       </c>
       <c r="B10" s="4">
         <f>SUM('Turma D'!O2:O50)/B7</f>
-        <v>0.6294642857142857</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="C10" s="4">
         <f>SUM('Turma E'!O2:O50)/C7</f>
@@ -4919,7 +4919,7 @@
       </c>
       <c r="F10" s="4">
         <f>AVERAGE(B10:E10)</f>
-        <v>0.68297371031746024</v>
+        <v>0.68632192460317465</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -5023,7 +5023,7 @@
       </c>
       <c r="B17" s="4">
         <f>SUM('Turma D'!E2:E50)/B6</f>
-        <v>0.45454545454545453</v>
+        <v>0.48484848484848486</v>
       </c>
       <c r="C17" s="4">
         <f>SUM('Turma E'!E2:E50)/C6</f>
@@ -5039,7 +5039,7 @@
       </c>
       <c r="F17" s="4">
         <f>AVERAGE(B17:E17)</f>
-        <v>0.49656080871659158</v>
+        <v>0.50413656629234915</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Ainda corrigindo o mesmo erro: número de RA duplicado na turma D
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagoa\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73F6EE4-F177-4A1E-8037-B1DC196B2C85}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F505524A-44AD-4717-A04D-8DFFEEBEAA10}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -858,7 +858,7 @@
                   <c:v>0.50197291562358437</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.50413656629234915</c:v>
+                  <c:v>0.49656080871659158</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1928,7 +1928,7 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2342,23 +2342,23 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>233901</v>
+        <v>233091</v>
       </c>
       <c r="B19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O19" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -2366,20 +2366,20 @@
         <v>233901</v>
       </c>
       <c r="B20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="10">
         <v>1</v>
       </c>
       <c r="O20" s="5">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -4878,7 +4878,7 @@
       </c>
       <c r="B9" s="4">
         <f>SUM('Turma D'!O2:O50)/B6</f>
-        <v>0.54545454545454541</v>
+        <v>0.53409090909090906</v>
       </c>
       <c r="C9" s="4">
         <f>SUM('Turma E'!O2:O50)/C6</f>
@@ -4894,7 +4894,7 @@
       </c>
       <c r="F9" s="4">
         <f>AVERAGE(B9:E9)</f>
-        <v>0.58056693011944782</v>
+        <v>0.57772602102853876</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -4903,7 +4903,7 @@
       </c>
       <c r="B10" s="4">
         <f>SUM('Turma D'!O2:O50)/B7</f>
-        <v>0.6428571428571429</v>
+        <v>0.6294642857142857</v>
       </c>
       <c r="C10" s="4">
         <f>SUM('Turma E'!O2:O50)/C7</f>
@@ -4919,7 +4919,7 @@
       </c>
       <c r="F10" s="4">
         <f>AVERAGE(B10:E10)</f>
-        <v>0.68632192460317465</v>
+        <v>0.68297371031746024</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -5023,7 +5023,7 @@
       </c>
       <c r="B17" s="4">
         <f>SUM('Turma D'!E2:E50)/B6</f>
-        <v>0.48484848484848486</v>
+        <v>0.45454545454545453</v>
       </c>
       <c r="C17" s="4">
         <f>SUM('Turma E'!E2:E50)/C6</f>
@@ -5039,7 +5039,7 @@
       </c>
       <c r="F17" s="4">
         <f>AVERAGE(B17:E17)</f>
-        <v>0.50413656629234915</v>
+        <v>0.49656080871659158</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Notas do lab 05 incluídas
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagoa\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F505524A-44AD-4717-A04D-8DFFEEBEAA10}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4836D5F2-F95C-428C-B568-71FD4B0E5691}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Turma D" sheetId="1" r:id="rId1"/>
@@ -824,9 +824,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Estatísticas!$A$14:$A$17</c:f>
+              <c:f>Estatísticas!$A$14:$A$18</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Lab 01</c:v>
                 </c:pt>
@@ -839,15 +839,18 @@
                 <c:pt idx="3">
                   <c:v>Lab 04</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>Lab 05</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Estatísticas!$F$14:$F$17</c:f>
+              <c:f>Estatísticas!$F$14:$F$18</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.81457573373387693</c:v>
                 </c:pt>
@@ -859,6 +862,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.49656080871659158</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.54101399518394011</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1927,8 +1933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1999,8 +2005,11 @@
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
       <c r="O2" s="5">
-        <f>(B2*1+C2*2+D2*2+E2*3)/8</f>
+        <f>(B2*1+C2*2+D2*2+E2*3+F2*3)/11</f>
         <v>1</v>
       </c>
     </row>
@@ -2020,9 +2029,12 @@
       <c r="E3">
         <v>0</v>
       </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O29" si="0">(B3*1+C3*2+D3*2+E3*3)/8</f>
-        <v>0.375</v>
+        <f t="shared" ref="O3:O29" si="0">(B3*1+C3*2+D3*2+E3*3+F3*3)/11</f>
+        <v>0.27272727272727271</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -2041,9 +2053,12 @@
       <c r="E4">
         <v>1</v>
       </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
       <c r="O4" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -2062,9 +2077,12 @@
       <c r="E5">
         <v>0</v>
       </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
       <c r="O5" s="5">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>0.27272727272727271</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -2083,9 +2101,12 @@
       <c r="E6">
         <v>1</v>
       </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
       <c r="O6" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -2104,9 +2125,12 @@
       <c r="E7">
         <v>0</v>
       </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
       <c r="O7" s="5">
         <f t="shared" si="0"/>
-        <v>0.625</v>
+        <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -2125,9 +2149,12 @@
       <c r="E8">
         <v>1</v>
       </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
       <c r="O8" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -2146,9 +2173,12 @@
       <c r="E9">
         <v>0</v>
       </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
       <c r="O9" s="5">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -2167,6 +2197,9 @@
       <c r="E10">
         <v>1</v>
       </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
       <c r="O10" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2188,9 +2221,12 @@
       <c r="E11">
         <v>0</v>
       </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
       <c r="O11" s="5">
         <f t="shared" si="0"/>
-        <v>0.625</v>
+        <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -2209,9 +2245,12 @@
       <c r="E12">
         <v>0</v>
       </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
       <c r="O12" s="5">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -2230,9 +2269,12 @@
       <c r="E13">
         <v>1</v>
       </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
       <c r="O13" s="5">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.81818181818181823</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -2251,6 +2293,9 @@
       <c r="E14">
         <v>1</v>
       </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
       <c r="O14" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2272,6 +2317,9 @@
       <c r="E15">
         <v>0</v>
       </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
       <c r="O15" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2293,6 +2341,9 @@
       <c r="E16">
         <v>1</v>
       </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
       <c r="O16" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2314,9 +2365,12 @@
       <c r="E17">
         <v>0</v>
       </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
       <c r="O17" s="5">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -2335,9 +2389,12 @@
       <c r="E18">
         <v>1</v>
       </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
       <c r="O18" s="5">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.81818181818181823</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -2356,6 +2413,9 @@
       <c r="E19">
         <v>0</v>
       </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
       <c r="O19" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2377,6 +2437,9 @@
       <c r="E20" s="10">
         <v>1</v>
       </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
       <c r="O20" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2398,9 +2461,12 @@
       <c r="E21">
         <v>0</v>
       </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
       <c r="O21" s="5">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>0.27272727272727271</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -2419,9 +2485,12 @@
       <c r="E22">
         <v>0</v>
       </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
       <c r="O22" s="5">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -2440,9 +2509,12 @@
       <c r="E23">
         <v>0</v>
       </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
       <c r="O23" s="5">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -2461,9 +2533,12 @@
       <c r="E24">
         <v>0</v>
       </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
       <c r="O24" s="5">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>0.27272727272727271</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -2482,9 +2557,12 @@
       <c r="E25">
         <v>1</v>
       </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
       <c r="O25" s="5">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.63636363636363635</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -2503,6 +2581,9 @@
       <c r="E26">
         <v>1</v>
       </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
       <c r="O26" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2524,9 +2605,12 @@
       <c r="E27">
         <v>1</v>
       </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
       <c r="O27" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
@@ -2545,6 +2629,9 @@
       <c r="E28">
         <v>1</v>
       </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
       <c r="O28" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2564,6 +2651,9 @@
         <v>1</v>
       </c>
       <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
         <v>1</v>
       </c>
       <c r="O29" s="5">
@@ -2664,9 +2754,12 @@
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
       <c r="O2" s="5">
-        <f>(B2*1+C2*2+D2*2+E2*3)/8</f>
-        <v>0.75</v>
+        <f>(B2*1+C2*2+D2*2+E2*3+F2*3)/11</f>
+        <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -2685,9 +2778,12 @@
       <c r="E3">
         <v>0</v>
       </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O25" si="0">(B3*1+C3*2+D3*2+E3*3)/8</f>
-        <v>0.625</v>
+        <f t="shared" ref="O3:O25" si="0">(B3*1+C3*2+D3*2+E3*3+F3*3)/11</f>
+        <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -2706,9 +2802,12 @@
       <c r="E4">
         <v>0</v>
       </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
       <c r="O4" s="5">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -2727,9 +2826,12 @@
       <c r="E5">
         <v>1</v>
       </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
       <c r="O5" s="5">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -2748,9 +2850,12 @@
       <c r="E6">
         <v>0</v>
       </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
       <c r="O6" s="5">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -2769,6 +2874,9 @@
       <c r="E7">
         <v>1</v>
       </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
       <c r="O7" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2790,9 +2898,12 @@
       <c r="E8">
         <v>0</v>
       </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
       <c r="O8" s="5">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -2811,9 +2922,12 @@
       <c r="E9">
         <v>0</v>
       </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
       <c r="O9" s="5">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -2832,6 +2946,9 @@
       <c r="E10">
         <v>1</v>
       </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
       <c r="O10" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2853,9 +2970,12 @@
       <c r="E11">
         <v>0</v>
       </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
       <c r="O11" s="5">
         <f t="shared" si="0"/>
-        <v>0.625</v>
+        <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -2874,6 +2994,9 @@
       <c r="E12">
         <v>1</v>
       </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
       <c r="O12" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2895,9 +3018,12 @@
       <c r="E13">
         <v>1</v>
       </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
       <c r="O13" s="5">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.81818181818181823</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -2916,6 +3042,9 @@
       <c r="E14">
         <v>1</v>
       </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
       <c r="O14" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2937,6 +3066,9 @@
       <c r="E15">
         <v>1</v>
       </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
       <c r="O15" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2958,6 +3090,9 @@
       <c r="E16">
         <v>1</v>
       </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
       <c r="O16" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2979,35 +3114,41 @@
       <c r="E17">
         <v>0</v>
       </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
       <c r="O17" s="5">
         <f t="shared" si="0"/>
-        <v>0.625</v>
+        <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>239253</v>
+        <v>237835</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
       </c>
       <c r="O18" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>239854</v>
+        <v>239253</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3019,6 +3160,9 @@
         <v>1</v>
       </c>
       <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
         <v>1</v>
       </c>
       <c r="O19" s="5">
@@ -3028,49 +3172,55 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>240259</v>
+        <v>239854</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
       </c>
       <c r="O20" s="5">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>240429</v>
+        <v>240259</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
       </c>
       <c r="O21" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>243070</v>
+        <v>240429</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3082,16 +3232,19 @@
         <v>1</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
       </c>
       <c r="O22" s="5">
         <f t="shared" si="0"/>
-        <v>0.625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>243472</v>
+        <v>243070</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3103,56 +3256,83 @@
         <v>1</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
       </c>
       <c r="O23" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.45454545454545453</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>243801</v>
+        <v>243472</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
       </c>
       <c r="O24" s="5">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
+        <v>243801</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="O25" s="5">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090912E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26">
         <v>257337</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="O25" s="5">
-        <f t="shared" si="0"/>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
       <c r="O26" s="5"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -3179,7 +3359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="O2" sqref="O2:O30"/>
     </sheetView>
   </sheetViews>
@@ -3248,9 +3428,12 @@
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
       <c r="O2" s="5">
-        <f>(B2*1+C2*2+D2*2+E2*3)/8</f>
-        <v>0.75</v>
+        <f>(B2*1+C2*2+D2*2+E2*3+F2*3)/11</f>
+        <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -3269,9 +3452,12 @@
       <c r="E3">
         <v>0</v>
       </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O30" si="0">(B3*1+C3*2+D3*2+E3*3)/8</f>
-        <v>0.125</v>
+        <f t="shared" ref="O3:O30" si="0">(B3*1+C3*2+D3*2+E3*3+F3*3)/11</f>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -3290,9 +3476,12 @@
       <c r="E4">
         <v>0</v>
       </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
       <c r="O4" s="5">
         <f t="shared" si="0"/>
-        <v>0.625</v>
+        <v>0.45454545454545453</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -3311,9 +3500,12 @@
       <c r="E5">
         <v>1</v>
       </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
       <c r="O5" s="5">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.81818181818181823</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -3332,9 +3524,12 @@
       <c r="E6">
         <v>0</v>
       </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
       <c r="O6" s="5">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>0.27272727272727271</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -3353,6 +3548,9 @@
       <c r="E7">
         <v>1</v>
       </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
       <c r="O7" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3374,6 +3572,9 @@
       <c r="E8">
         <v>1</v>
       </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
       <c r="O8" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3395,9 +3596,12 @@
       <c r="E9">
         <v>0</v>
       </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
       <c r="O9" s="5">
         <f t="shared" si="0"/>
-        <v>0.625</v>
+        <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -3416,9 +3620,12 @@
       <c r="E10">
         <v>0</v>
       </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
       <c r="O10" s="5">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -3437,6 +3644,9 @@
       <c r="E11">
         <v>1</v>
       </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
       <c r="O11" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3458,6 +3668,9 @@
       <c r="E12">
         <v>1</v>
       </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
       <c r="O12" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3479,6 +3692,9 @@
       <c r="E13">
         <v>0</v>
       </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
       <c r="O13" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3500,9 +3716,12 @@
       <c r="E14">
         <v>1</v>
       </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
       <c r="O14" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -3521,6 +3740,9 @@
       <c r="E15">
         <v>1</v>
       </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
       <c r="O15" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3542,6 +3764,9 @@
       <c r="E16">
         <v>1</v>
       </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
       <c r="O16" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3563,6 +3788,9 @@
       <c r="E17">
         <v>1</v>
       </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
       <c r="O17" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3584,9 +3812,12 @@
       <c r="E18">
         <v>0</v>
       </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
       <c r="O18" s="5">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.18181818181818182</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -3605,9 +3836,12 @@
       <c r="E19">
         <v>0</v>
       </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
       <c r="O19" s="5">
         <f t="shared" si="0"/>
-        <v>0.625</v>
+        <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -3626,6 +3860,9 @@
       <c r="E20">
         <v>1</v>
       </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
       <c r="O20" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3647,6 +3884,9 @@
       <c r="E21">
         <v>1</v>
       </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
       <c r="O21" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3668,6 +3908,9 @@
       <c r="E22">
         <v>1</v>
       </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
       <c r="O22" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3689,9 +3932,12 @@
       <c r="E23">
         <v>0</v>
       </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
       <c r="O23" s="5">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -3710,6 +3956,9 @@
       <c r="E24">
         <v>1</v>
       </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
       <c r="O24" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3731,6 +3980,9 @@
       <c r="E25">
         <v>1</v>
       </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
       <c r="O25" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3752,6 +4004,9 @@
       <c r="E26">
         <v>1</v>
       </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
       <c r="O26" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3773,6 +4028,9 @@
       <c r="E27">
         <v>1</v>
       </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
       <c r="O27" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3794,6 +4052,9 @@
       <c r="E28">
         <v>1</v>
       </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
       <c r="O28" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3815,9 +4076,12 @@
       <c r="E29">
         <v>0</v>
       </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
       <c r="O29" s="5">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -3834,6 +4098,9 @@
         <v>1</v>
       </c>
       <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
         <v>1</v>
       </c>
       <c r="O30" s="5">
@@ -3862,8 +4129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3931,9 +4198,12 @@
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
       <c r="O2" s="5">
-        <f>(B2*1+C2*2+D2*2+E2*3)/8</f>
-        <v>0.75</v>
+        <f>(B2*1+C2*2+D2*2+E2*3+F2*3)/11</f>
+        <v>0.81818181818181823</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -3952,9 +4222,12 @@
       <c r="E3">
         <v>0</v>
       </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O37" si="0">(B3*1+C3*2+D3*2+E3*3)/8</f>
-        <v>0.125</v>
+        <f t="shared" ref="O3:O37" si="0">(B3*1+C3*2+D3*2+E3*3+F3*3)/11</f>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -3973,9 +4246,12 @@
       <c r="E4">
         <v>0</v>
       </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
       <c r="O4" s="5">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>0.27272727272727271</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -3994,9 +4270,12 @@
       <c r="E5">
         <v>1</v>
       </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
       <c r="O5" s="5">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.81818181818181823</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -4015,9 +4294,12 @@
       <c r="E6">
         <v>0</v>
       </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
       <c r="O6" s="5">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -4036,6 +4318,9 @@
       <c r="E7">
         <v>1</v>
       </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
       <c r="O7" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4057,6 +4342,9 @@
       <c r="E8">
         <v>1</v>
       </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
       <c r="O8" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4078,9 +4366,12 @@
       <c r="E9">
         <v>0</v>
       </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
       <c r="O9" s="5">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -4099,9 +4390,12 @@
       <c r="E10">
         <v>1</v>
       </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
       <c r="O10" s="5">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.81818181818181823</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -4120,6 +4414,9 @@
       <c r="E11">
         <v>1</v>
       </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
       <c r="O11" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4141,9 +4438,12 @@
       <c r="E12">
         <v>1</v>
       </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
       <c r="O12" s="5">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.81818181818181823</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -4162,9 +4462,12 @@
       <c r="E13">
         <v>0</v>
       </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
       <c r="O13" s="5">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>0.27272727272727271</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -4183,9 +4486,12 @@
       <c r="E14">
         <v>1</v>
       </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
       <c r="O14" s="5">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.81818181818181823</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -4204,6 +4510,9 @@
       <c r="E15">
         <v>1</v>
       </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
       <c r="O15" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4225,9 +4534,12 @@
       <c r="E16">
         <v>0</v>
       </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
       <c r="O16" s="5">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>0.27272727272727271</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -4246,9 +4558,12 @@
       <c r="E17">
         <v>1</v>
       </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
       <c r="O17" s="5">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.81818181818181823</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -4267,6 +4582,9 @@
       <c r="E18">
         <v>1</v>
       </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
       <c r="O18" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4288,6 +4606,9 @@
       <c r="E19">
         <v>1</v>
       </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
       <c r="O19" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4309,6 +4630,9 @@
       <c r="E20">
         <v>1</v>
       </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
       <c r="O20" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4330,6 +4654,9 @@
       <c r="E21">
         <v>1</v>
       </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
       <c r="O21" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4351,9 +4678,12 @@
       <c r="E22">
         <v>1</v>
       </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
       <c r="O22" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -4372,6 +4702,9 @@
       <c r="E23">
         <v>1</v>
       </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
       <c r="O23" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4393,9 +4726,12 @@
       <c r="E24">
         <v>0</v>
       </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
       <c r="O24" s="5">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -4414,6 +4750,9 @@
       <c r="E25">
         <v>1</v>
       </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
       <c r="O25" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4435,9 +4774,12 @@
       <c r="E26">
         <v>1</v>
       </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
       <c r="O26" s="5">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.81818181818181823</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -4456,6 +4798,9 @@
       <c r="E27">
         <v>1</v>
       </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
       <c r="O27" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4477,9 +4822,12 @@
       <c r="E28">
         <v>0</v>
       </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
       <c r="O28" s="5">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>0.27272727272727271</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -4498,9 +4846,12 @@
       <c r="E29">
         <v>0</v>
       </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
       <c r="O29" s="5">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -4519,9 +4870,12 @@
       <c r="E30">
         <v>0</v>
       </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
       <c r="O30" s="5">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>0.36363636363636365</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -4540,9 +4894,12 @@
       <c r="E31">
         <v>0</v>
       </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
       <c r="O31" s="5">
         <f t="shared" si="0"/>
-        <v>0.625</v>
+        <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
@@ -4561,9 +4918,12 @@
       <c r="E32">
         <v>0</v>
       </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
       <c r="O32" s="5">
         <f t="shared" si="0"/>
-        <v>0.625</v>
+        <v>0.45454545454545453</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
@@ -4582,9 +4942,12 @@
       <c r="E33">
         <v>0</v>
       </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
       <c r="O33" s="5">
         <f t="shared" si="0"/>
-        <v>0.625</v>
+        <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
@@ -4603,6 +4966,9 @@
       <c r="E34">
         <v>1</v>
       </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
       <c r="O34" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4624,6 +4990,9 @@
       <c r="E35">
         <v>1</v>
       </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
       <c r="O35" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4645,6 +5014,9 @@
       <c r="E36">
         <v>1</v>
       </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
       <c r="O36" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4666,9 +5038,12 @@
       <c r="E37">
         <v>0</v>
       </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
       <c r="O37" s="5">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4692,8 +5067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4832,7 +5207,7 @@
       </c>
       <c r="C7">
         <f>COUNTA('Turma E'!A2:A50)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <f>COUNTA('Turma F'!A2:A50)</f>
@@ -4844,7 +5219,7 @@
       </c>
       <c r="F7">
         <f>SUM(B7:E7)</f>
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -4857,7 +5232,7 @@
       </c>
       <c r="C8" s="4">
         <f t="shared" ref="C8:F8" si="0">(C7/C6)</f>
-        <v>0.77419354838709675</v>
+        <v>0.80645161290322576</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="0"/>
@@ -4869,7 +5244,7 @@
       </c>
       <c r="F8" s="4">
         <f t="shared" si="0"/>
-        <v>0.84782608695652173</v>
+        <v>0.85507246376811596</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -4878,23 +5253,23 @@
       </c>
       <c r="B9" s="4">
         <f>SUM('Turma D'!O2:O50)/B6</f>
-        <v>0.53409090909090906</v>
+        <v>0.50413223140495877</v>
       </c>
       <c r="C9" s="4">
         <f>SUM('Turma E'!O2:O50)/C6</f>
-        <v>0.52016129032258063</v>
+        <v>0.5161290322580645</v>
       </c>
       <c r="D9" s="4">
         <f>SUM('Turma F'!O2:O50)/D6</f>
-        <v>0.65909090909090906</v>
+        <v>0.64462809917355368</v>
       </c>
       <c r="E9" s="4">
         <f>SUM('Turma G'!O2:O50)/E6</f>
-        <v>0.59756097560975607</v>
+        <v>0.5942350332594234</v>
       </c>
       <c r="F9" s="4">
         <f>AVERAGE(B9:E9)</f>
-        <v>0.57772602102853876</v>
+        <v>0.56478109902400009</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -4903,23 +5278,23 @@
       </c>
       <c r="B10" s="4">
         <f>SUM('Turma D'!O2:O50)/B7</f>
-        <v>0.6294642857142857</v>
+        <v>0.59415584415584433</v>
       </c>
       <c r="C10" s="4">
         <f>SUM('Turma E'!O2:O50)/C7</f>
-        <v>0.671875</v>
+        <v>0.64</v>
       </c>
       <c r="D10" s="4">
         <f>SUM('Turma F'!O2:O50)/D7</f>
-        <v>0.75</v>
+        <v>0.73354231974921624</v>
       </c>
       <c r="E10" s="4">
         <f>SUM('Turma G'!O2:O50)/E7</f>
-        <v>0.68055555555555558</v>
+        <v>0.67676767676767668</v>
       </c>
       <c r="F10" s="4">
         <f>AVERAGE(B10:E10)</f>
-        <v>0.68297371031746024</v>
+        <v>0.66111646016818426</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -5045,6 +5420,26 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>15</v>
+      </c>
+      <c r="B18" s="4">
+        <f>SUM('Turma D'!F2:F50)/B6</f>
+        <v>0.42424242424242425</v>
+      </c>
+      <c r="C18" s="4">
+        <f>SUM('Turma E'!F2:F50)/C6</f>
+        <v>0.54838709677419351</v>
+      </c>
+      <c r="D18" s="4">
+        <f>SUM('Turma F'!F2:F50)/D6</f>
+        <v>0.60606060606060608</v>
+      </c>
+      <c r="E18" s="4">
+        <f>SUM('Turma G'!F2:F50)/E6</f>
+        <v>0.58536585365853655</v>
+      </c>
+      <c r="F18" s="4">
+        <f>AVERAGE(B18:E18)</f>
+        <v>0.54101399518394011</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Notas dos labs 07 e 09
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagoa\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4836D5F2-F95C-428C-B568-71FD4B0E5691}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F04566-7BF8-47DD-92D2-9FA2E46A974B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Turma G" sheetId="4" r:id="rId4"/>
     <sheet name="Estatísticas" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="27">
   <si>
     <t>RA</t>
   </si>
@@ -823,34 +823,11 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:strRef>
-              <c:f>Estatísticas!$A$14:$A$18</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Lab 01</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Lab 02</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Lab 03</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Lab 04</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Lab 05</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
             <c:numRef>
-              <c:f>Estatísticas!$F$14:$F$18</c:f>
+              <c:f>(Estatísticas!$F$14,Estatísticas!$F$15,Estatísticas!$F$16,Estatísticas!$F$17,Estatísticas!$F$18,Estatísticas!$F$20,Estatísticas!$F$22)</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.81457573373387693</c:v>
                 </c:pt>
@@ -865,6 +842,42 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.54101399518394011</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.62878787878787878</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.59090909090909083</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Estatísticas!$F$14,Estatísticas!$F$15,Estatísticas!$F$16,Estatísticas!$F$17,Estatísticas!$F$18,Estatísticas!$F$20,Estatísticas!$F$22)</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.81457573373387693</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.65680208854874478</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.50197291562358437</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.49656080871659158</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.54101399518394011</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.62878787878787878</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.59090909090909083</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -896,7 +909,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1934,7 +1947,7 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2008,8 +2021,14 @@
       <c r="F2">
         <v>1</v>
       </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
       <c r="O2" s="5">
-        <f>(B2*1+C2*2+D2*2+E2*3+F2*3)/11</f>
+        <f>(B2*1+C2*2+D2*2+E2*3+F2*3+H2*3+J2*3)/17</f>
         <v>1</v>
       </c>
     </row>
@@ -2032,9 +2051,15 @@
       <c r="F3">
         <v>0</v>
       </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O29" si="0">(B3*1+C3*2+D3*2+E3*3+F3*3)/11</f>
-        <v>0.27272727272727271</v>
+        <f t="shared" ref="O3:O29" si="0">(B3*1+C3*2+D3*2+E3*3+F3*3+H3*3+J3*3)/17</f>
+        <v>0.17647058823529413</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -2056,9 +2081,15 @@
       <c r="F4">
         <v>0</v>
       </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
       <c r="O4" s="5">
         <f t="shared" si="0"/>
-        <v>0.72727272727272729</v>
+        <v>0.47058823529411764</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -2080,9 +2111,15 @@
       <c r="F5">
         <v>0</v>
       </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
       <c r="O5" s="5">
         <f t="shared" si="0"/>
-        <v>0.27272727272727271</v>
+        <v>0.17647058823529413</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -2104,9 +2141,15 @@
       <c r="F6">
         <v>0</v>
       </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
       <c r="O6" s="5">
         <f t="shared" si="0"/>
-        <v>0.72727272727272729</v>
+        <v>0.47058823529411764</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -2128,9 +2171,15 @@
       <c r="F7">
         <v>1</v>
       </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
       <c r="O7" s="5">
         <f t="shared" si="0"/>
-        <v>0.72727272727272729</v>
+        <v>0.82352941176470584</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -2152,9 +2201,15 @@
       <c r="F8">
         <v>0</v>
       </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
       <c r="O8" s="5">
         <f t="shared" si="0"/>
-        <v>0.72727272727272729</v>
+        <v>0.6470588235294118</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -2176,9 +2231,15 @@
       <c r="F9">
         <v>0</v>
       </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
       <c r="O9" s="5">
         <f t="shared" si="0"/>
-        <v>9.0909090909090912E-2</v>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -2200,6 +2261,12 @@
       <c r="F10">
         <v>1</v>
       </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
       <c r="O10" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2224,9 +2291,15 @@
       <c r="F11">
         <v>1</v>
       </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
       <c r="O11" s="5">
         <f t="shared" si="0"/>
-        <v>0.72727272727272729</v>
+        <v>0.6470588235294118</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -2248,9 +2321,15 @@
       <c r="F12">
         <v>0</v>
       </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
       <c r="O12" s="5">
         <f t="shared" si="0"/>
-        <v>9.0909090909090912E-2</v>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -2272,9 +2351,15 @@
       <c r="F13">
         <v>1</v>
       </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
       <c r="O13" s="5">
         <f t="shared" si="0"/>
-        <v>0.81818181818181823</v>
+        <v>0.88235294117647056</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -2296,6 +2381,12 @@
       <c r="F14">
         <v>1</v>
       </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
       <c r="O14" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2320,9 +2411,15 @@
       <c r="F15">
         <v>0</v>
       </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
       <c r="O15" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.35294117647058826</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -2344,9 +2441,15 @@
       <c r="F16">
         <v>1</v>
       </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
       <c r="O16" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.6470588235294118</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -2368,9 +2471,15 @@
       <c r="F17">
         <v>1</v>
       </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
       <c r="O17" s="5">
         <f t="shared" si="0"/>
-        <v>0.54545454545454541</v>
+        <v>0.70588235294117652</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -2392,9 +2501,15 @@
       <c r="F18">
         <v>1</v>
       </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
       <c r="O18" s="5">
         <f t="shared" si="0"/>
-        <v>0.81818181818181823</v>
+        <v>0.88235294117647056</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -2416,9 +2531,15 @@
       <c r="F19">
         <v>0</v>
       </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
       <c r="O19" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.17647058823529413</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -2440,6 +2561,12 @@
       <c r="F20">
         <v>1</v>
       </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
       <c r="O20" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2464,9 +2591,15 @@
       <c r="F21">
         <v>0</v>
       </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
       <c r="O21" s="5">
         <f t="shared" si="0"/>
-        <v>0.27272727272727271</v>
+        <v>0.17647058823529413</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -2488,9 +2621,15 @@
       <c r="F22">
         <v>0</v>
       </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
       <c r="O22" s="5">
         <f t="shared" si="0"/>
-        <v>9.0909090909090912E-2</v>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -2512,9 +2651,15 @@
       <c r="F23">
         <v>0</v>
       </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
       <c r="O23" s="5">
         <f t="shared" si="0"/>
-        <v>9.0909090909090912E-2</v>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -2536,9 +2681,15 @@
       <c r="F24">
         <v>0</v>
       </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
       <c r="O24" s="5">
         <f t="shared" si="0"/>
-        <v>0.27272727272727271</v>
+        <v>0.35294117647058826</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -2560,9 +2711,15 @@
       <c r="F25">
         <v>1</v>
       </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
       <c r="O25" s="5">
         <f t="shared" si="0"/>
-        <v>0.63636363636363635</v>
+        <v>0.76470588235294112</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -2584,6 +2741,12 @@
       <c r="F26">
         <v>1</v>
       </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
       <c r="O26" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2608,9 +2771,15 @@
       <c r="F27">
         <v>0</v>
       </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
       <c r="O27" s="5">
         <f t="shared" si="0"/>
-        <v>0.72727272727272729</v>
+        <v>0.6470588235294118</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
@@ -2632,6 +2801,12 @@
       <c r="F28">
         <v>1</v>
       </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
       <c r="O28" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2654,6 +2829,12 @@
         <v>1</v>
       </c>
       <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="J29">
         <v>1</v>
       </c>
       <c r="O29" s="5">
@@ -2685,7 +2866,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O25"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2740,31 +2921,37 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>155452</v>
+        <v>116003</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
       <c r="O2" s="5">
-        <f>(B2*1+C2*2+D2*2+E2*3+F2*3)/11</f>
+        <f>(B3*1+C3*2+D3*2+E3*3+F3*3)/11</f>
         <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>174929</v>
+        <v>155452</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2773,46 +2960,58 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>1</v>
       </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O25" si="0">(B3*1+C3*2+D3*2+E3*3+F3*3)/11</f>
+        <f>(B4*1+C4*2+D4*2+E4*3+F4*3)/11</f>
         <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>184293</v>
+        <v>174929</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
       </c>
       <c r="O4" s="5">
-        <f t="shared" si="0"/>
+        <f>(B5*1+C5*2+D5*2+E5*3+F5*3)/11</f>
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>186289</v>
+        <v>184293</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2821,46 +3020,58 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
       <c r="O5" s="5">
-        <f t="shared" si="0"/>
+        <f>(B6*1+C6*2+D6*2+E6*3+F6*3)/11</f>
         <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>199883</v>
+        <v>186289</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
       </c>
       <c r="O6" s="5">
-        <f t="shared" si="0"/>
+        <f>(B7*1+C7*2+D7*2+E7*3+F7*3)/11</f>
         <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>201270</v>
+        <v>199883</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2869,22 +3080,28 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
       <c r="O7" s="5">
-        <f t="shared" si="0"/>
+        <f>(B8*1+C8*2+D8*2+E8*3+F8*3)/11</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>216097</v>
+        <v>201270</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2893,28 +3110,34 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
       <c r="O8" s="5">
-        <f t="shared" si="0"/>
+        <f>(B9*1+C9*2+D9*2+E9*3+F9*3)/11</f>
         <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>218861</v>
+        <v>216097</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -2923,40 +3146,52 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
       </c>
       <c r="O9" s="5">
-        <f t="shared" si="0"/>
+        <f>(B10*1+C10*2+D10*2+E10*3+F10*3)/11</f>
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>220728</v>
+        <v>218861</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
       </c>
       <c r="O10" s="5">
-        <f t="shared" si="0"/>
+        <f>(B11*1+C11*2+D11*2+E11*3+F11*3)/11</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>221040</v>
+        <v>220728</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2968,19 +3203,25 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
       <c r="O11" s="5">
-        <f t="shared" si="0"/>
+        <f>(B12*1+C12*2+D12*2+E12*3+F12*3)/11</f>
         <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>222523</v>
+        <v>221040</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -2992,19 +3233,25 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
       <c r="O12" s="5">
-        <f t="shared" si="0"/>
+        <f>(B13*1+C13*2+D13*2+E13*3+F13*3)/11</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>223280</v>
+        <v>222523</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3013,7 +3260,7 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -3021,14 +3268,20 @@
       <c r="F13">
         <v>1</v>
       </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
       <c r="O13" s="5">
-        <f t="shared" si="0"/>
+        <f>(B14*1+C14*2+D14*2+E14*3+F14*3)/11</f>
         <v>0.81818181818181823</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>223346</v>
+        <v>223280</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3037,7 +3290,7 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -3045,14 +3298,20 @@
       <c r="F14">
         <v>1</v>
       </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
       <c r="O14" s="5">
-        <f t="shared" si="0"/>
+        <f>(B15*1+C15*2+D15*2+E15*3+F15*3)/11</f>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>223849</v>
+        <v>223346</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3069,14 +3328,20 @@
       <c r="F15">
         <v>1</v>
       </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
       <c r="O15" s="5">
-        <f t="shared" si="0"/>
+        <f>(B16*1+C16*2+D16*2+E16*3+F16*3)/11</f>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>234589</v>
+        <v>223849</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3093,14 +3358,20 @@
       <c r="F16">
         <v>1</v>
       </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
       <c r="O16" s="5">
-        <f t="shared" si="0"/>
+        <f>(B17*1+C17*2+D17*2+E17*3+F17*3)/11</f>
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>237402</v>
+        <v>234589</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3112,67 +3383,85 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
       <c r="O17" s="5">
-        <f t="shared" si="0"/>
+        <f>(B18*1+C18*2+D18*2+E18*3+F18*3)/11</f>
         <v>0.72727272727272729</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>237835</v>
+        <v>237402</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
       </c>
       <c r="O18" s="5">
-        <f t="shared" si="0"/>
+        <f>(B19*1+C19*2+D19*2+E19*3+F19*3)/11</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>239253</v>
+        <v>237835</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
       </c>
       <c r="O19" s="5">
-        <f t="shared" si="0"/>
+        <f>(B20*1+C20*2+D20*2+E20*3+F20*3)/11</f>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>239854</v>
+        <v>239253</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3189,62 +3478,80 @@
       <c r="F20">
         <v>1</v>
       </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
       <c r="O20" s="5">
-        <f t="shared" si="0"/>
+        <f>(B21*1+C21*2+D21*2+E21*3+F21*3)/11</f>
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>240259</v>
+        <v>239854</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
       </c>
       <c r="O21" s="5">
-        <f t="shared" si="0"/>
+        <f>(B22*1+C22*2+D22*2+E22*3+F22*3)/11</f>
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>240429</v>
+        <v>240259</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="J22">
         <v>1</v>
       </c>
       <c r="O22" s="5">
-        <f t="shared" si="0"/>
+        <f>(B23*1+C23*2+D23*2+E23*3+F23*3)/11</f>
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>243070</v>
+        <v>240429</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3256,19 +3563,25 @@
         <v>1</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
       </c>
       <c r="O23" s="5">
-        <f t="shared" si="0"/>
+        <f>(B24*1+C24*2+D24*2+E24*3+F24*3)/11</f>
         <v>0.45454545454545453</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>243472</v>
+        <v>243070</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3280,62 +3593,107 @@
         <v>1</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="J24">
         <v>1</v>
       </c>
       <c r="O24" s="5">
-        <f t="shared" si="0"/>
+        <f>(B25*1+C25*2+D25*2+E25*3+F25*3)/11</f>
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>243801</v>
+        <v>243472</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
       </c>
       <c r="O25" s="5">
-        <f t="shared" si="0"/>
+        <f>(B26*1+C26*2+D26*2+E26*3+F26*3)/11</f>
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26">
+        <v>243801</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="O26" s="5">
+        <f>(B27*1+C27*2+D27*2+E27*3+F27*3)/11</f>
+        <v>0.36363636363636365</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27">
         <v>257337</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="O26" s="5"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
       <c r="O27" s="5"/>
     </row>
   </sheetData>
@@ -3359,8 +3717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3431,9 +3789,15 @@
       <c r="F2">
         <v>0</v>
       </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
       <c r="O2" s="5">
-        <f>(B2*1+C2*2+D2*2+E2*3+F2*3)/11</f>
-        <v>0.54545454545454541</v>
+        <f>(B2*1+C2*2+D2*2+E2*3+F2*3+H2*3+J2*3)/17</f>
+        <v>0.35294117647058826</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -3455,9 +3819,15 @@
       <c r="F3">
         <v>0</v>
       </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O30" si="0">(B3*1+C3*2+D3*2+E3*3+F3*3)/11</f>
-        <v>9.0909090909090912E-2</v>
+        <f t="shared" ref="O3:O30" si="0">(B3*1+C3*2+D3*2+E3*3+F3*3+H3*3+J3*3)/17</f>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -3479,9 +3849,15 @@
       <c r="F4">
         <v>0</v>
       </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
       <c r="O4" s="5">
         <f t="shared" si="0"/>
-        <v>0.45454545454545453</v>
+        <v>0.47058823529411764</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -3503,9 +3879,15 @@
       <c r="F5">
         <v>1</v>
       </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
       <c r="O5" s="5">
         <f t="shared" si="0"/>
-        <v>0.81818181818181823</v>
+        <v>0.88235294117647056</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -3527,9 +3909,15 @@
       <c r="F6">
         <v>0</v>
       </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
       <c r="O6" s="5">
         <f t="shared" si="0"/>
-        <v>0.27272727272727271</v>
+        <v>0.17647058823529413</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -3551,6 +3939,12 @@
       <c r="F7">
         <v>1</v>
       </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
       <c r="O7" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3575,6 +3969,12 @@
       <c r="F8">
         <v>1</v>
       </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
       <c r="O8" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3599,9 +3999,15 @@
       <c r="F9">
         <v>1</v>
       </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
       <c r="O9" s="5">
         <f t="shared" si="0"/>
-        <v>0.72727272727272729</v>
+        <v>0.6470588235294118</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -3623,9 +4029,15 @@
       <c r="F10">
         <v>0</v>
       </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
       <c r="O10" s="5">
         <f t="shared" si="0"/>
-        <v>9.0909090909090912E-2</v>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -3647,6 +4059,12 @@
       <c r="F11">
         <v>1</v>
       </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
       <c r="O11" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3671,6 +4089,12 @@
       <c r="F12">
         <v>1</v>
       </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
       <c r="O12" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3695,6 +4119,12 @@
       <c r="F13">
         <v>0</v>
       </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
       <c r="O13" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3719,9 +4149,15 @@
       <c r="F14">
         <v>0</v>
       </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
       <c r="O14" s="5">
         <f t="shared" si="0"/>
-        <v>0.72727272727272729</v>
+        <v>0.47058823529411764</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -3743,6 +4179,12 @@
       <c r="F15">
         <v>1</v>
       </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
       <c r="O15" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3767,6 +4209,12 @@
       <c r="F16">
         <v>1</v>
       </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
       <c r="O16" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3791,6 +4239,12 @@
       <c r="F17">
         <v>1</v>
       </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
       <c r="O17" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3815,9 +4269,15 @@
       <c r="F18">
         <v>0</v>
       </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
       <c r="O18" s="5">
         <f t="shared" si="0"/>
-        <v>0.18181818181818182</v>
+        <v>0.29411764705882354</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -3839,9 +4299,15 @@
       <c r="F19">
         <v>1</v>
       </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
       <c r="O19" s="5">
         <f t="shared" si="0"/>
-        <v>0.72727272727272729</v>
+        <v>0.82352941176470584</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -3863,6 +4329,12 @@
       <c r="F20">
         <v>1</v>
       </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
       <c r="O20" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3887,6 +4359,12 @@
       <c r="F21">
         <v>1</v>
       </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
       <c r="O21" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3911,9 +4389,15 @@
       <c r="F22">
         <v>1</v>
       </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
       <c r="O22" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.82352941176470584</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -3935,9 +4419,15 @@
       <c r="F23">
         <v>1</v>
       </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
       <c r="O23" s="5">
         <f t="shared" si="0"/>
-        <v>0.54545454545454541</v>
+        <v>0.52941176470588236</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -3959,6 +4449,12 @@
       <c r="F24">
         <v>1</v>
       </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
       <c r="O24" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3983,6 +4479,12 @@
       <c r="F25">
         <v>1</v>
       </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
       <c r="O25" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4007,6 +4509,12 @@
       <c r="F26">
         <v>1</v>
       </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
       <c r="O26" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4031,6 +4539,12 @@
       <c r="F27">
         <v>1</v>
       </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
       <c r="O27" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4055,6 +4569,12 @@
       <c r="F28">
         <v>1</v>
       </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
       <c r="O28" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4079,9 +4599,15 @@
       <c r="F29">
         <v>0</v>
       </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
       <c r="O29" s="5">
         <f t="shared" si="0"/>
-        <v>9.0909090909090912E-2</v>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -4101,6 +4627,12 @@
         <v>1</v>
       </c>
       <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="J30">
         <v>1</v>
       </c>
       <c r="O30" s="5">
@@ -4129,8 +4661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4201,9 +4733,15 @@
       <c r="F2">
         <v>1</v>
       </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
       <c r="O2" s="5">
-        <f>(B2*1+C2*2+D2*2+E2*3+F2*3)/11</f>
-        <v>0.81818181818181823</v>
+        <f>(B2*1+C2*2+D2*2+E2*3+F2*3+H2*3+J2*3)/17</f>
+        <v>0.88235294117647056</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -4225,9 +4763,15 @@
       <c r="F3">
         <v>0</v>
       </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O37" si="0">(B3*1+C3*2+D3*2+E3*3+F3*3)/11</f>
-        <v>9.0909090909090912E-2</v>
+        <f t="shared" ref="O3:O37" si="0">(B3*1+C3*2+D3*2+E3*3+F3*3+H3*3+J3*3)/17</f>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -4249,9 +4793,15 @@
       <c r="F4">
         <v>0</v>
       </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
       <c r="O4" s="5">
         <f t="shared" si="0"/>
-        <v>0.27272727272727271</v>
+        <v>0.17647058823529413</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -4273,9 +4823,15 @@
       <c r="F5">
         <v>1</v>
       </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
       <c r="O5" s="5">
         <f t="shared" si="0"/>
-        <v>0.81818181818181823</v>
+        <v>0.88235294117647056</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -4297,9 +4853,15 @@
       <c r="F6">
         <v>0</v>
       </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
       <c r="O6" s="5">
         <f t="shared" si="0"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.41176470588235292</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -4321,6 +4883,12 @@
       <c r="F7">
         <v>1</v>
       </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
       <c r="O7" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4345,6 +4913,12 @@
       <c r="F8">
         <v>1</v>
       </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
       <c r="O8" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4369,9 +4943,15 @@
       <c r="F9">
         <v>0</v>
       </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
       <c r="O9" s="5">
         <f t="shared" si="0"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.41176470588235292</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -4393,9 +4973,15 @@
       <c r="F10">
         <v>1</v>
       </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
       <c r="O10" s="5">
         <f t="shared" si="0"/>
-        <v>0.81818181818181823</v>
+        <v>0.88235294117647056</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -4417,6 +5003,12 @@
       <c r="F11">
         <v>1</v>
       </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
       <c r="O11" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4441,9 +5033,15 @@
       <c r="F12">
         <v>1</v>
       </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
       <c r="O12" s="5">
         <f t="shared" si="0"/>
-        <v>0.81818181818181823</v>
+        <v>0.88235294117647056</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -4465,9 +5063,15 @@
       <c r="F13">
         <v>0</v>
       </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
       <c r="O13" s="5">
         <f t="shared" si="0"/>
-        <v>0.27272727272727271</v>
+        <v>0.17647058823529413</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -4489,9 +5093,15 @@
       <c r="F14">
         <v>1</v>
       </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
       <c r="O14" s="5">
         <f t="shared" si="0"/>
-        <v>0.81818181818181823</v>
+        <v>0.88235294117647056</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -4513,6 +5123,12 @@
       <c r="F15">
         <v>1</v>
       </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
       <c r="O15" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4537,9 +5153,15 @@
       <c r="F16">
         <v>0</v>
       </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
       <c r="O16" s="5">
         <f t="shared" si="0"/>
-        <v>0.27272727272727271</v>
+        <v>0.17647058823529413</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -4561,9 +5183,15 @@
       <c r="F17">
         <v>1</v>
       </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
       <c r="O17" s="5">
         <f t="shared" si="0"/>
-        <v>0.81818181818181823</v>
+        <v>0.70588235294117652</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -4585,6 +5213,12 @@
       <c r="F18">
         <v>1</v>
       </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
       <c r="O18" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4609,6 +5243,12 @@
       <c r="F19">
         <v>1</v>
       </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
       <c r="O19" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4633,6 +5273,12 @@
       <c r="F20">
         <v>1</v>
       </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
       <c r="O20" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4657,6 +5303,12 @@
       <c r="F21">
         <v>1</v>
       </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
       <c r="O21" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4681,9 +5333,15 @@
       <c r="F22">
         <v>0</v>
       </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
       <c r="O22" s="5">
         <f t="shared" si="0"/>
-        <v>0.72727272727272729</v>
+        <v>0.6470588235294118</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -4705,6 +5363,12 @@
       <c r="F23">
         <v>1</v>
       </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
       <c r="O23" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4729,9 +5393,15 @@
       <c r="F24">
         <v>0</v>
       </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
       <c r="O24" s="5">
         <f t="shared" si="0"/>
-        <v>9.0909090909090912E-2</v>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -4753,6 +5423,12 @@
       <c r="F25">
         <v>1</v>
       </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
       <c r="O25" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4777,9 +5453,15 @@
       <c r="F26">
         <v>1</v>
       </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
       <c r="O26" s="5">
         <f t="shared" si="0"/>
-        <v>0.81818181818181823</v>
+        <v>0.70588235294117652</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -4801,6 +5483,12 @@
       <c r="F27">
         <v>1</v>
       </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
       <c r="O27" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4825,9 +5513,15 @@
       <c r="F28">
         <v>0</v>
       </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
       <c r="O28" s="5">
         <f t="shared" si="0"/>
-        <v>0.27272727272727271</v>
+        <v>0.35294117647058826</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -4849,9 +5543,15 @@
       <c r="F29">
         <v>0</v>
       </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
       <c r="O29" s="5">
         <f t="shared" si="0"/>
-        <v>9.0909090909090912E-2</v>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -4873,9 +5573,15 @@
       <c r="F30">
         <v>1</v>
       </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
       <c r="O30" s="5">
         <f t="shared" si="0"/>
-        <v>0.36363636363636365</v>
+        <v>0.58823529411764708</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -4897,9 +5603,15 @@
       <c r="F31">
         <v>1</v>
       </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
       <c r="O31" s="5">
         <f t="shared" si="0"/>
-        <v>0.72727272727272729</v>
+        <v>0.82352941176470584</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
@@ -4921,9 +5633,15 @@
       <c r="F32">
         <v>0</v>
       </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
       <c r="O32" s="5">
         <f t="shared" si="0"/>
-        <v>0.45454545454545453</v>
+        <v>0.29411764705882354</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
@@ -4945,9 +5663,15 @@
       <c r="F33">
         <v>1</v>
       </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
       <c r="O33" s="5">
         <f t="shared" si="0"/>
-        <v>0.72727272727272729</v>
+        <v>0.82352941176470584</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
@@ -4969,6 +5693,12 @@
       <c r="F34">
         <v>1</v>
       </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
       <c r="O34" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4993,6 +5723,12 @@
       <c r="F35">
         <v>1</v>
       </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
       <c r="O35" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5017,6 +5753,12 @@
       <c r="F36">
         <v>1</v>
       </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
       <c r="O36" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5041,9 +5783,15 @@
       <c r="F37">
         <v>0</v>
       </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
       <c r="O37" s="5">
         <f t="shared" si="0"/>
-        <v>9.0909090909090912E-2</v>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
   </sheetData>
@@ -5068,15 +5816,15 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -5143,11 +5891,11 @@
       <c r="H2" s="2">
         <v>3</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>23</v>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
+        <v>3</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>23</v>
@@ -5206,7 +5954,7 @@
         <v>28</v>
       </c>
       <c r="C7">
-        <f>COUNTA('Turma E'!A2:A50)</f>
+        <f>COUNTA('Turma E'!A3:A50)</f>
         <v>25</v>
       </c>
       <c r="D7">
@@ -5253,23 +6001,23 @@
       </c>
       <c r="B9" s="4">
         <f>SUM('Turma D'!O2:O50)/B6</f>
-        <v>0.50413223140495877</v>
+        <v>0.49197860962566842</v>
       </c>
       <c r="C9" s="4">
         <f>SUM('Turma E'!O2:O50)/C6</f>
-        <v>0.5161290322580645</v>
+        <v>0.52785923753665687</v>
       </c>
       <c r="D9" s="4">
         <f>SUM('Turma F'!O2:O50)/D6</f>
-        <v>0.64462809917355368</v>
+        <v>0.62566844919786102</v>
       </c>
       <c r="E9" s="4">
         <f>SUM('Turma G'!O2:O50)/E6</f>
-        <v>0.5942350332594234</v>
+        <v>0.60832137733142033</v>
       </c>
       <c r="F9" s="4">
         <f>AVERAGE(B9:E9)</f>
-        <v>0.56478109902400009</v>
+        <v>0.56345691842290169</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -5278,23 +6026,23 @@
       </c>
       <c r="B10" s="4">
         <f>SUM('Turma D'!O2:O50)/B7</f>
-        <v>0.59415584415584433</v>
+        <v>0.57983193277310918</v>
       </c>
       <c r="C10" s="4">
         <f>SUM('Turma E'!O2:O50)/C7</f>
-        <v>0.64</v>
+        <v>0.65454545454545454</v>
       </c>
       <c r="D10" s="4">
         <f>SUM('Turma F'!O2:O50)/D7</f>
-        <v>0.73354231974921624</v>
+        <v>0.71196754563894527</v>
       </c>
       <c r="E10" s="4">
         <f>SUM('Turma G'!O2:O50)/E7</f>
-        <v>0.67676767676767668</v>
+        <v>0.69281045751633985</v>
       </c>
       <c r="F10" s="4">
         <f>AVERAGE(B10:E10)</f>
-        <v>0.66111646016818426</v>
+        <v>0.65978884761846213</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -5326,7 +6074,7 @@
         <v>0.78787878787878785</v>
       </c>
       <c r="C14" s="4">
-        <f>SUM('Turma E'!B2:B50)/C6</f>
+        <f>SUM('Turma E'!B3:B50)/C6</f>
         <v>0.77419354838709675</v>
       </c>
       <c r="D14" s="4">
@@ -5351,7 +6099,7 @@
         <v>0.63636363636363635</v>
       </c>
       <c r="C15" s="4">
-        <f>SUM('Turma E'!C2:C50)/C6</f>
+        <f>SUM('Turma E'!C3:C50)/C6</f>
         <v>0.58064516129032262</v>
       </c>
       <c r="D15" s="4">
@@ -5376,7 +6124,7 @@
         <v>0.42424242424242425</v>
       </c>
       <c r="C16" s="4">
-        <f>SUM('Turma E'!D2:D50)/C6</f>
+        <f>SUM('Turma E'!D3:D50)/C6</f>
         <v>0.4838709677419355</v>
       </c>
       <c r="D16" s="4">
@@ -5401,7 +6149,7 @@
         <v>0.45454545454545453</v>
       </c>
       <c r="C17" s="4">
-        <f>SUM('Turma E'!E2:E50)/C6</f>
+        <f>SUM('Turma E'!E3:E50)/C6</f>
         <v>0.41935483870967744</v>
       </c>
       <c r="D17" s="4">
@@ -5426,7 +6174,7 @@
         <v>0.42424242424242425</v>
       </c>
       <c r="C18" s="4">
-        <f>SUM('Turma E'!F2:F50)/C6</f>
+        <f>SUM('Turma E'!F3:F50)/C6</f>
         <v>0.54838709677419351</v>
       </c>
       <c r="D18" s="4">
@@ -5446,20 +6194,66 @@
       <c r="A19" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="B20" s="4">
+        <f>SUM('Turma D'!H2:H50)/B6</f>
+        <v>0.51515151515151514</v>
+      </c>
+      <c r="C20" s="4">
+        <f>SUM('Turma E'!H2:H50)/B6</f>
+        <v>0.5757575757575758</v>
+      </c>
+      <c r="D20" s="4">
+        <f>SUM('Turma F'!H2:H50)/B6</f>
+        <v>0.60606060606060608</v>
+      </c>
+      <c r="E20" s="4">
+        <f>SUM('Turma G'!H2:H50)/B6</f>
+        <v>0.81818181818181823</v>
+      </c>
+      <c r="F20" s="4">
+        <f t="shared" ref="F19:F22" si="1">AVERAGE(B20:E20)</f>
+        <v>0.62878787878787878</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>18</v>
       </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>19</v>
+      </c>
+      <c r="B22" s="4">
+        <f>SUM('Turma D'!J2:J50)/B6</f>
+        <v>0.42424242424242425</v>
+      </c>
+      <c r="C22" s="4">
+        <f>SUM('Turma E'!J2:J50)/B6</f>
+        <v>0.60606060606060608</v>
+      </c>
+      <c r="D22" s="4">
+        <f>SUM('Turma F'!J2:J50)/B6</f>
+        <v>0.5757575757575758</v>
+      </c>
+      <c r="E22" s="4">
+        <f>SUM('Turma G'!J2:J50)/B6</f>
+        <v>0.75757575757575757</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" si="1"/>
+        <v>0.59090909090909083</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Corrigido um erro no somatório das notas da turma E
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagoa\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F04566-7BF8-47DD-92D2-9FA2E46A974B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2DA026-FABF-40CF-9E76-DECAEF1EB760}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Turma D" sheetId="1" r:id="rId1"/>
@@ -1946,8 +1946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2866,7 +2866,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2945,8 +2945,8 @@
         <v>0</v>
       </c>
       <c r="O2" s="5">
-        <f>(B3*1+C3*2+D3*2+E3*3+F3*3)/11</f>
-        <v>0.54545454545454541</v>
+        <f>(B2*1+C2*2+D2*2+E2*3+F2*3+H2*3+J2*3)/17</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -2975,8 +2975,8 @@
         <v>1</v>
       </c>
       <c r="O3" s="5">
-        <f>(B4*1+C4*2+D4*2+E4*3+F4*3)/11</f>
-        <v>0.72727272727272729</v>
+        <f t="shared" ref="O3:O27" si="0">(B3*1+C3*2+D3*2+E3*3+F3*3+H3*3+J3*3)/17</f>
+        <v>0.70588235294117652</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -3005,8 +3005,8 @@
         <v>1</v>
       </c>
       <c r="O4" s="5">
-        <f>(B5*1+C5*2+D5*2+E5*3+F5*3)/11</f>
-        <v>9.0909090909090912E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.82352941176470584</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -3035,8 +3035,8 @@
         <v>0</v>
       </c>
       <c r="O5" s="5">
-        <f>(B6*1+C6*2+D6*2+E6*3+F6*3)/11</f>
-        <v>0.54545454545454541</v>
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -3065,8 +3065,8 @@
         <v>0</v>
       </c>
       <c r="O6" s="5">
-        <f>(B7*1+C7*2+D7*2+E7*3+F7*3)/11</f>
-        <v>0.54545454545454541</v>
+        <f t="shared" si="0"/>
+        <v>0.35294117647058826</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -3095,8 +3095,8 @@
         <v>1</v>
       </c>
       <c r="O7" s="5">
-        <f>(B8*1+C8*2+D8*2+E8*3+F8*3)/11</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.70588235294117652</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -3125,8 +3125,8 @@
         <v>1</v>
       </c>
       <c r="O8" s="5">
-        <f>(B9*1+C9*2+D9*2+E9*3+F9*3)/11</f>
-        <v>0.54545454545454541</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -3155,8 +3155,8 @@
         <v>1</v>
       </c>
       <c r="O9" s="5">
-        <f>(B10*1+C10*2+D10*2+E10*3+F10*3)/11</f>
-        <v>9.0909090909090912E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.70588235294117652</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -3185,8 +3185,8 @@
         <v>0</v>
       </c>
       <c r="O10" s="5">
-        <f>(B11*1+C11*2+D11*2+E11*3+F11*3)/11</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -3215,8 +3215,8 @@
         <v>1</v>
       </c>
       <c r="O11" s="5">
-        <f>(B12*1+C12*2+D12*2+E12*3+F12*3)/11</f>
-        <v>0.72727272727272729</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -3245,8 +3245,8 @@
         <v>1</v>
       </c>
       <c r="O12" s="5">
-        <f>(B13*1+C13*2+D13*2+E13*3+F13*3)/11</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.82352941176470584</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -3275,8 +3275,8 @@
         <v>1</v>
       </c>
       <c r="O13" s="5">
-        <f>(B14*1+C14*2+D14*2+E14*3+F14*3)/11</f>
-        <v>0.81818181818181823</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -3305,8 +3305,8 @@
         <v>1</v>
       </c>
       <c r="O14" s="5">
-        <f>(B15*1+C15*2+D15*2+E15*3+F15*3)/11</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.88235294117647056</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -3335,7 +3335,7 @@
         <v>1</v>
       </c>
       <c r="O15" s="5">
-        <f>(B16*1+C16*2+D16*2+E16*3+F16*3)/11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3365,7 +3365,7 @@
         <v>1</v>
       </c>
       <c r="O16" s="5">
-        <f>(B17*1+C17*2+D17*2+E17*3+F17*3)/11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3395,8 +3395,8 @@
         <v>1</v>
       </c>
       <c r="O17" s="5">
-        <f>(B18*1+C18*2+D18*2+E18*3+F18*3)/11</f>
-        <v>0.72727272727272729</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -3425,8 +3425,8 @@
         <v>1</v>
       </c>
       <c r="O18" s="5">
-        <f>(B19*1+C19*2+D19*2+E19*3+F19*3)/11</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.82352941176470584</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -3455,8 +3455,8 @@
         <v>0</v>
       </c>
       <c r="O19" s="5">
-        <f>(B20*1+C20*2+D20*2+E20*3+F20*3)/11</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -3485,7 +3485,7 @@
         <v>1</v>
       </c>
       <c r="O20" s="5">
-        <f>(B21*1+C21*2+D21*2+E21*3+F21*3)/11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3515,8 +3515,8 @@
         <v>1</v>
       </c>
       <c r="O21" s="5">
-        <f>(B22*1+C22*2+D22*2+E22*3+F22*3)/11</f>
-        <v>9.0909090909090912E-2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -3545,8 +3545,8 @@
         <v>1</v>
       </c>
       <c r="O22" s="5">
-        <f>(B23*1+C23*2+D23*2+E23*3+F23*3)/11</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.23529411764705882</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -3575,8 +3575,8 @@
         <v>1</v>
       </c>
       <c r="O23" s="5">
-        <f>(B24*1+C24*2+D24*2+E24*3+F24*3)/11</f>
-        <v>0.45454545454545453</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -3605,8 +3605,8 @@
         <v>1</v>
       </c>
       <c r="O24" s="5">
-        <f>(B25*1+C25*2+D25*2+E25*3+F25*3)/11</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.6470588235294118</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -3635,8 +3635,8 @@
         <v>1</v>
       </c>
       <c r="O25" s="5">
-        <f>(B26*1+C26*2+D26*2+E26*3+F26*3)/11</f>
-        <v>9.0909090909090912E-2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -3665,8 +3665,8 @@
         <v>0</v>
       </c>
       <c r="O26" s="5">
-        <f>(B27*1+C27*2+D27*2+E27*3+F27*3)/11</f>
-        <v>0.36363636363636365</v>
+        <f t="shared" si="0"/>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -3694,7 +3694,10 @@
       <c r="J27">
         <v>1</v>
       </c>
-      <c r="O27" s="5"/>
+      <c r="O27" s="5">
+        <f t="shared" si="0"/>
+        <v>0.58823529411764708</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="O2:O27">
@@ -3718,7 +3721,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4662,7 +4665,7 @@
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5815,7 +5818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -6005,7 +6008,7 @@
       </c>
       <c r="C9" s="4">
         <f>SUM('Turma E'!O2:O50)/C6</f>
-        <v>0.52785923753665687</v>
+        <v>0.56356736242884242</v>
       </c>
       <c r="D9" s="4">
         <f>SUM('Turma F'!O2:O50)/D6</f>
@@ -6017,7 +6020,7 @@
       </c>
       <c r="F9" s="4">
         <f>AVERAGE(B9:E9)</f>
-        <v>0.56345691842290169</v>
+        <v>0.57238394964594808</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -6030,7 +6033,7 @@
       </c>
       <c r="C10" s="4">
         <f>SUM('Turma E'!O2:O50)/C7</f>
-        <v>0.65454545454545454</v>
+        <v>0.69882352941176462</v>
       </c>
       <c r="D10" s="4">
         <f>SUM('Turma F'!O2:O50)/D7</f>
@@ -6042,7 +6045,7 @@
       </c>
       <c r="F10" s="4">
         <f>AVERAGE(B10:E10)</f>
-        <v>0.65978884761846213</v>
+        <v>0.67085836633503981</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -6217,7 +6220,7 @@
         <v>0.81818181818181823</v>
       </c>
       <c r="F20" s="4">
-        <f t="shared" ref="F19:F22" si="1">AVERAGE(B20:E20)</f>
+        <f t="shared" ref="F20:F22" si="1">AVERAGE(B20:E20)</f>
         <v>0.62878787878787878</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Notas finais, contando as entregas atrasadas
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagoa\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2DA026-FABF-40CF-9E76-DECAEF1EB760}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817F7F79-DAC8-4C6D-BAF0-EE0B3C87BCE5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Turma D" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="28">
   <si>
     <t>RA</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Lab 12</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>nota média/inscritos</t>
   </si>
   <si>
@@ -112,6 +109,12 @@
   </si>
   <si>
     <t># entregas</t>
+  </si>
+  <si>
+    <t># aprovados (sem exame)</t>
+  </si>
+  <si>
+    <t>aprovados (sem exame) (%)</t>
   </si>
 </sst>
 </file>
@@ -626,7 +629,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -657,6 +660,7 @@
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -703,7 +707,68 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -750,13 +815,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="pt-BR"/>
-              <a:t>Entregas</a:t>
+              <a:rPr lang="pt-BR" sz="1600" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Entregas com sucesso de cada lab (% de alunos)</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="pt-BR" baseline="0"/>
-              <a:t> com sucesso de cada lab (% de alunos)</a:t>
-            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1600">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -796,12 +862,12 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:idx val="4"/>
+          <c:order val="4"/>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -814,7 +880,7 @@
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:ln w="38100">
+              <a:ln w="19050">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -823,61 +889,86 @@
             </c:spPr>
           </c:marker>
           <c:cat>
-            <c:numRef>
-              <c:f>(Estatísticas!$F$14,Estatísticas!$F$15,Estatísticas!$F$16,Estatísticas!$F$17,Estatísticas!$F$18,Estatísticas!$F$20,Estatísticas!$F$22)</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="7"/>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Estatísticas!$A$16:$A$27</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Estatísticas!$A$16:$A$20,Estatísticas!$A$22,Estatísticas!$A$24:$A$25,Estatísticas!$A$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.81457573373387693</c:v>
+                  <c:v>Lab 01</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.65680208854874478</c:v>
+                  <c:v>Lab 02</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.50197291562358437</c:v>
+                  <c:v>Lab 03</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.49656080871659158</c:v>
+                  <c:v>Lab 04</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.54101399518394011</c:v>
+                  <c:v>Lab 05</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.62878787878787878</c:v>
+                  <c:v>Lab 07</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.59090909090909083</c:v>
+                  <c:v>Lab 09</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+                <c:pt idx="7">
+                  <c:v>Lab 10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Lab 12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Estatísticas!$F$14,Estatísticas!$F$15,Estatísticas!$F$16,Estatísticas!$F$17,Estatísticas!$F$18,Estatísticas!$F$20,Estatísticas!$F$22)</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Estatísticas!$F$16:$F$27</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Estatísticas!$F$16:$F$20,Estatísticas!$F$22,Estatísticas!$F$24:$F$25,Estatísticas!$F$27)</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.81457573373387693</c:v>
+                  <c:v>0.849033211739742</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.65680208854874478</c:v>
+                  <c:v>0.70645429511479874</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.50197291562358437</c:v>
+                  <c:v>0.56224668001811984</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.49656080871659158</c:v>
+                  <c:v>0.55115275492930882</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.54101399518394011</c:v>
+                  <c:v>0.61796664520897415</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.62878787878787878</c:v>
+                  <c:v>0.68721240731468891</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.59090909090909083</c:v>
+                  <c:v>0.63264430298261931</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.68721240731468891</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.19240397682569202</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -885,7 +976,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B5F7-4164-A043-217B11EAF733}"/>
+              <c16:uniqueId val="{00000004-1550-4A39-B040-1C8A24A9EB54}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -899,17 +990,521 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1132646320"/>
-        <c:axId val="889854544"/>
+        <c:axId val="1323120000"/>
+        <c:axId val="1018798256"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Estatísticas!$A$16:$A$27</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(Estatísticas!$A$16:$A$20,Estatísticas!$A$22,Estatísticas!$A$24:$A$25,Estatísticas!$A$27)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>Lab 01</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Lab 02</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Lab 03</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Lab 04</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Lab 05</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Lab 07</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Lab 09</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Lab 10</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Lab 12</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Estatísticas!$B$16:$B$27</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(Estatísticas!$B$16:$B$20,Estatísticas!$B$22,Estatísticas!$B$24:$B$25,Estatísticas!$B$27)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0%</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>0.83333333333333337</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.68181818181818177</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.46969696969696972</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.47727272727272729</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.53787878787878785</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.62878787878787878</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.53787878787878785</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.62878787878787878</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.18181818181818182</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-1550-4A39-B040-1C8A24A9EB54}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Estatísticas!$A$16:$A$27</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(Estatísticas!$A$16:$A$20,Estatísticas!$A$22,Estatísticas!$A$24:$A$25,Estatísticas!$A$27)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>Lab 01</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Lab 02</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Lab 03</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Lab 04</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Lab 05</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Lab 07</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Lab 09</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Lab 10</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Lab 12</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Estatísticas!$C$16:$C$27</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(Estatísticas!$C$16:$C$20,Estatísticas!$C$22,Estatísticas!$C$24:$C$25,Estatísticas!$C$27)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0%</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>0.79838709677419351</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.62903225806451613</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.55645161290322576</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.49193548387096775</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.59677419354838712</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.70967741935483875</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.69354838709677424</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.70967741935483875</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>6.4516129032258063E-2</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-1550-4A39-B040-1C8A24A9EB54}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Estatísticas!$A$16:$A$27</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(Estatísticas!$A$16:$A$20,Estatísticas!$A$22,Estatísticas!$A$24:$A$25,Estatísticas!$A$27)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>Lab 01</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Lab 02</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Lab 03</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Lab 04</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Lab 05</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Lab 07</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Lab 09</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Lab 10</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Lab 12</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Estatísticas!$D$16:$D$27</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(Estatísticas!$D$16:$D$20,Estatísticas!$D$22,Estatísticas!$D$24:$D$25,Estatísticas!$D$27)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0%</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>0.88636363636363635</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.79545454545454541</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.70454545454545459</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.64393939393939392</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.69696969696969702</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.69696969696969702</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.68939393939393945</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.69696969696969702</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.18181818181818182</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-1550-4A39-B040-1C8A24A9EB54}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Estatísticas!$A$16:$A$27</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(Estatísticas!$A$16:$A$20,Estatísticas!$A$22,Estatísticas!$A$24:$A$25,Estatísticas!$A$27)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>Lab 01</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Lab 02</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Lab 03</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Lab 04</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Lab 05</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Lab 07</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Lab 09</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Lab 10</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Lab 12</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>Estatísticas!$E$16:$E$27</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>(Estatísticas!$E$16:$E$20,Estatísticas!$E$22,Estatísticas!$E$24:$E$25,Estatísticas!$E$27)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0%</c:formatCode>
+                      <c:ptCount val="9"/>
+                      <c:pt idx="0">
+                        <c:v>0.87804878048780488</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.71951219512195119</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.51829268292682928</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.59146341463414631</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.6402439024390244</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.71341463414634143</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.6097560975609756</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.71341463414634143</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.34146341463414637</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-1550-4A39-B040-1C8A24A9EB54}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1132646320"/>
+        <c:axId val="1323120000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -931,7 +1526,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -946,7 +1541,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="889854544"/>
+        <c:crossAx val="1018798256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -954,7 +1549,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="889854544"/>
+        <c:axId val="1018798256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -974,10 +1569,10 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="low"/>
+        <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
@@ -990,7 +1585,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1005,7 +1600,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1132646320"/>
+        <c:crossAx val="1323120000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1610,23 +2205,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>179070</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>281940</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59CF201E-8D08-4B8E-BA5B-A2F1C2300535}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8833980E-F375-47BD-9EF6-F26AA7533DC0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1946,8 +2541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2027,8 +2622,14 @@
       <c r="J2">
         <v>1</v>
       </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
       <c r="O2" s="5">
-        <f>(B2*1+C2*2+D2*2+E2*3+F2*3+H2*3+J2*3)/17</f>
+        <f>(B2*1+C2*2+D2*2+E2*3+F2*3+H2*3+J2*3+K2*4+M2*4)/25</f>
         <v>1</v>
       </c>
     </row>
@@ -2057,9 +2658,15 @@
       <c r="J3">
         <v>0</v>
       </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O29" si="0">(B3*1+C3*2+D3*2+E3*3+F3*3+H3*3+J3*3)/17</f>
-        <v>0.17647058823529413</v>
+        <f t="shared" ref="O3:O29" si="0">(B3*1+C3*2+D3*2+E3*3+F3*3+H3*3+J3*3+K3*4+M3*4)/25</f>
+        <v>0.12</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -2079,17 +2686,23 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>0.75</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
       </c>
       <c r="O4" s="5">
         <f t="shared" si="0"/>
-        <v>0.47058823529411764</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -2117,9 +2730,15 @@
       <c r="J5">
         <v>0</v>
       </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
       <c r="O5" s="5">
         <f t="shared" si="0"/>
-        <v>0.17647058823529413</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -2142,14 +2761,20 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J6">
+        <v>0.75</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="M6">
         <v>0</v>
       </c>
       <c r="O6" s="5">
         <f t="shared" si="0"/>
-        <v>0.47058823529411764</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -2177,9 +2802,15 @@
       <c r="J7">
         <v>1</v>
       </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
       <c r="O7" s="5">
         <f t="shared" si="0"/>
-        <v>0.82352941176470584</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -2199,17 +2830,23 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="J8">
+        <v>0.75</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="M8">
         <v>0</v>
       </c>
       <c r="O8" s="5">
         <f t="shared" si="0"/>
-        <v>0.6470588235294118</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -2229,17 +2866,23 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>0.75</v>
+      </c>
+      <c r="K9">
+        <v>0.75</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
       </c>
       <c r="O9" s="5">
         <f t="shared" si="0"/>
-        <v>5.8823529411764705E-2</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -2267,9 +2910,15 @@
       <c r="J10">
         <v>1</v>
       </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
       <c r="O10" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -2297,9 +2946,15 @@
       <c r="J11">
         <v>0</v>
       </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
       <c r="O11" s="5">
         <f t="shared" si="0"/>
-        <v>0.6470588235294118</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -2327,9 +2982,15 @@
       <c r="J12">
         <v>0</v>
       </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
       <c r="O12" s="5">
         <f t="shared" si="0"/>
-        <v>5.8823529411764705E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -2357,9 +3018,15 @@
       <c r="J13">
         <v>1</v>
       </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
       <c r="O13" s="5">
         <f t="shared" si="0"/>
-        <v>0.88235294117647056</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -2387,9 +3054,15 @@
       <c r="J14">
         <v>1</v>
       </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
       <c r="O14" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -2397,7 +3070,7 @@
         <v>221215</v>
       </c>
       <c r="B15" s="2">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="C15" s="2">
         <v>0</v>
@@ -2409,7 +3082,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -2417,9 +3090,15 @@
       <c r="J15">
         <v>1</v>
       </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
       <c r="O15" s="5">
         <f t="shared" si="0"/>
-        <v>0.35294117647058826</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -2442,14 +3121,20 @@
         <v>1</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
       <c r="O16" s="5">
         <f t="shared" si="0"/>
-        <v>0.6470588235294118</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -2477,9 +3162,15 @@
       <c r="J17">
         <v>1</v>
       </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
       <c r="O17" s="5">
         <f t="shared" si="0"/>
-        <v>0.70588235294117652</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -2507,9 +3198,15 @@
       <c r="J18">
         <v>1</v>
       </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
       <c r="O18" s="5">
         <f t="shared" si="0"/>
-        <v>0.88235294117647056</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -2517,29 +3214,35 @@
         <v>233091</v>
       </c>
       <c r="B19" s="2">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="C19" s="2">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="D19" s="2">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J19">
         <v>1</v>
       </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
       <c r="O19" s="5">
         <f t="shared" si="0"/>
-        <v>0.17647058823529413</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -2567,6 +3270,12 @@
       <c r="J20">
         <v>1</v>
       </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
       <c r="O20" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2597,9 +3306,15 @@
       <c r="J21">
         <v>0</v>
       </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
       <c r="O21" s="5">
         <f t="shared" si="0"/>
-        <v>0.17647058823529413</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -2627,9 +3342,15 @@
       <c r="J22">
         <v>0</v>
       </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
       <c r="O22" s="5">
         <f t="shared" si="0"/>
-        <v>5.8823529411764705E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -2657,9 +3378,15 @@
       <c r="J23">
         <v>0</v>
       </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
       <c r="O23" s="5">
         <f t="shared" si="0"/>
-        <v>5.8823529411764705E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -2687,9 +3414,15 @@
       <c r="J24">
         <v>0</v>
       </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
       <c r="O24" s="5">
         <f t="shared" si="0"/>
-        <v>0.35294117647058826</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -2700,10 +3433,10 @@
         <v>1</v>
       </c>
       <c r="C25" s="2">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="D25" s="2">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -2717,9 +3450,15 @@
       <c r="J25">
         <v>1</v>
       </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
       <c r="O25" s="5">
         <f t="shared" si="0"/>
-        <v>0.76470588235294112</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -2747,9 +3486,15 @@
       <c r="J26">
         <v>1</v>
       </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
       <c r="O26" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -2775,11 +3520,17 @@
         <v>1</v>
       </c>
       <c r="J27">
+        <v>0.75</v>
+      </c>
+      <c r="K27">
+        <v>0.75</v>
+      </c>
+      <c r="M27">
         <v>0</v>
       </c>
       <c r="O27" s="5">
         <f t="shared" si="0"/>
-        <v>0.6470588235294118</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
@@ -2807,9 +3558,15 @@
       <c r="J28">
         <v>1</v>
       </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
       <c r="O28" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -2837,6 +3594,12 @@
       <c r="J29">
         <v>1</v>
       </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
       <c r="O29" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2845,7 +3608,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="O2:O29">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.5"/>
@@ -2866,7 +3629,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2924,10 +3687,10 @@
         <v>116003</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -2936,17 +3699,23 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
+      <c r="K2">
+        <v>0.75</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
       <c r="O2" s="5">
-        <f>(B2*1+C2*2+D2*2+E2*3+F2*3+H2*3+J2*3)/17</f>
-        <v>0</v>
+        <f>(B2*1+C2*2+D2*2+E2*3+F2*3+H2*3+J2*3+K2*4+M2*4)/25</f>
+        <v>0.39</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -2960,7 +3729,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2974,9 +3743,15 @@
       <c r="J3">
         <v>1</v>
       </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O27" si="0">(B3*1+C3*2+D3*2+E3*3+F3*3+H3*3+J3*3)/17</f>
-        <v>0.70588235294117652</v>
+        <f t="shared" ref="O3:O27" si="0">(B3*1+C3*2+D3*2+E3*3+F3*3+H3*3+J3*3+K3*4+M3*4)/25</f>
+        <v>0.7</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -3004,9 +3779,15 @@
       <c r="J4">
         <v>1</v>
       </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
       <c r="O4" s="5">
         <f t="shared" si="0"/>
-        <v>0.82352941176470584</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -3034,9 +3815,15 @@
       <c r="J5">
         <v>0</v>
       </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
       <c r="O5" s="5">
         <f t="shared" si="0"/>
-        <v>5.8823529411764705E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -3059,14 +3846,20 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J6">
+        <v>0.75</v>
+      </c>
+      <c r="K6">
+        <v>0.75</v>
+      </c>
+      <c r="M6">
         <v>0</v>
       </c>
       <c r="O6" s="5">
         <f t="shared" si="0"/>
-        <v>0.35294117647058826</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -3080,10 +3873,10 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -3094,9 +3887,15 @@
       <c r="J7">
         <v>1</v>
       </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
       <c r="O7" s="5">
         <f t="shared" si="0"/>
-        <v>0.70588235294117652</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -3124,9 +3923,15 @@
       <c r="J8">
         <v>1</v>
       </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
       <c r="O8" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -3140,10 +3945,10 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -3154,9 +3959,15 @@
       <c r="J9">
         <v>1</v>
       </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
       <c r="O9" s="5">
         <f t="shared" si="0"/>
-        <v>0.70588235294117652</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -3184,9 +3995,15 @@
       <c r="J10">
         <v>0</v>
       </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
       <c r="O10" s="5">
         <f t="shared" si="0"/>
-        <v>5.8823529411764705E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -3214,9 +4031,15 @@
       <c r="J11">
         <v>1</v>
       </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
       <c r="O11" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -3244,9 +4067,15 @@
       <c r="J12">
         <v>1</v>
       </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
       <c r="O12" s="5">
         <f t="shared" si="0"/>
-        <v>0.82352941176470584</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -3274,9 +4103,15 @@
       <c r="J13">
         <v>1</v>
       </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
       <c r="O13" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -3304,9 +4139,15 @@
       <c r="J14">
         <v>1</v>
       </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
       <c r="O14" s="5">
         <f t="shared" si="0"/>
-        <v>0.88235294117647056</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -3334,9 +4175,15 @@
       <c r="J15">
         <v>1</v>
       </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
       <c r="O15" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -3364,9 +4211,15 @@
       <c r="J16">
         <v>1</v>
       </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
       <c r="O16" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -3394,9 +4247,15 @@
       <c r="J17">
         <v>1</v>
       </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
       <c r="O17" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -3424,9 +4283,15 @@
       <c r="J18">
         <v>1</v>
       </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
       <c r="O18" s="5">
         <f t="shared" si="0"/>
-        <v>0.82352941176470584</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -3434,29 +4299,35 @@
         <v>237835</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J19">
+        <v>0.75</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="M19">
         <v>0</v>
       </c>
       <c r="O19" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -3484,6 +4355,12 @@
       <c r="J20">
         <v>1</v>
       </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
       <c r="O20" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -3514,9 +4391,15 @@
       <c r="J21">
         <v>1</v>
       </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
       <c r="O21" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -3536,17 +4419,23 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J22">
         <v>1</v>
       </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
       <c r="O22" s="5">
         <f t="shared" si="0"/>
-        <v>0.23529411764705882</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -3574,9 +4463,15 @@
       <c r="J23">
         <v>1</v>
       </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
       <c r="O23" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -3596,7 +4491,7 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -3604,9 +4499,15 @@
       <c r="J24">
         <v>1</v>
       </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
       <c r="O24" s="5">
         <f t="shared" si="0"/>
-        <v>0.6470588235294118</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -3634,9 +4535,15 @@
       <c r="J25">
         <v>1</v>
       </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
       <c r="O25" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -3664,9 +4571,15 @@
       <c r="J26">
         <v>0</v>
       </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
       <c r="O26" s="5">
         <f t="shared" si="0"/>
-        <v>5.8823529411764705E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -3677,7 +4590,7 @@
         <v>1</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -3694,14 +4607,20 @@
       <c r="J27">
         <v>1</v>
       </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
       <c r="O27" s="5">
         <f t="shared" si="0"/>
-        <v>0.58823529411764708</v>
+        <v>0.62</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="O2:O27">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.5"/>
@@ -3712,16 +4631,21 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B27">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3798,9 +4722,15 @@
       <c r="J2">
         <v>0</v>
       </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
       <c r="O2" s="5">
-        <f>(B2*1+C2*2+D2*2+E2*3+F2*3+H2*3+J2*3)/17</f>
-        <v>0.35294117647058826</v>
+        <f>(B2*1+C2*2+D2*2+E2*3+F2*3+H2*3+J2*3+K2*4+M2*4)/25</f>
+        <v>0.24</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -3828,9 +4758,15 @@
       <c r="J3">
         <v>0</v>
       </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O30" si="0">(B3*1+C3*2+D3*2+E3*3+F3*3+H3*3+J3*3)/17</f>
-        <v>5.8823529411764705E-2</v>
+        <f t="shared" ref="O3:O31" si="0">(B3*1+C3*2+D3*2+E3*3+F3*3+H3*3+J3*3+K3*4+M3*4)/25</f>
+        <v>0.04</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -3850,52 +4786,64 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
+      <c r="K4">
+        <v>0.75</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
       <c r="O4" s="5">
         <f t="shared" si="0"/>
-        <v>0.47058823529411764</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>195216</v>
+        <v>176573</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0.75</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
       </c>
       <c r="O5" s="5">
         <f t="shared" si="0"/>
-        <v>0.88235294117647056</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>196419</v>
+        <v>195216</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3904,28 +4852,34 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="M6">
         <v>0</v>
       </c>
       <c r="O6" s="5">
         <f t="shared" si="0"/>
-        <v>0.17647058823529413</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>200025</v>
+        <v>196419</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3934,28 +4888,34 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
       </c>
       <c r="O7" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>203904</v>
+        <v>200025</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3976,6 +4936,12 @@
         <v>1</v>
       </c>
       <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="M8">
         <v>1</v>
       </c>
       <c r="O8" s="5">
@@ -3985,7 +4951,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>204299</v>
+        <v>203904</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3997,7 +4963,7 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -4006,76 +4972,94 @@
         <v>1</v>
       </c>
       <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="M9">
         <v>0</v>
       </c>
       <c r="O9" s="5">
         <f t="shared" si="0"/>
-        <v>0.6470588235294118</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>204820</v>
+        <v>204299</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
+        <v>0.75</v>
+      </c>
+      <c r="K10">
+        <v>0.75</v>
+      </c>
+      <c r="M10">
         <v>0</v>
       </c>
       <c r="O10" s="5">
         <f t="shared" si="0"/>
-        <v>5.8823529411764705E-2</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>212234</v>
+        <v>204820</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
       </c>
       <c r="O11" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>213259</v>
+        <v>212234</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -4096,6 +5080,12 @@
         <v>1</v>
       </c>
       <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="M12">
         <v>1</v>
       </c>
       <c r="O12" s="5">
@@ -4105,67 +5095,79 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>213356</v>
+        <v>213259</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="M13">
         <v>0</v>
       </c>
       <c r="O13" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>214321</v>
+        <v>213356</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J14">
+        <v>0.75</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="M14">
         <v>0</v>
       </c>
       <c r="O14" s="5">
         <f t="shared" si="0"/>
-        <v>0.47058823529411764</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>217276</v>
+        <v>214321</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -4180,22 +5182,28 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
       </c>
       <c r="O15" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>222298</v>
+        <v>217276</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -4216,6 +5224,12 @@
         <v>1</v>
       </c>
       <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="M16">
         <v>1</v>
       </c>
       <c r="O16" s="5">
@@ -4225,7 +5239,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>232235</v>
+        <v>222298</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -4248,74 +5262,92 @@
       <c r="J17">
         <v>1</v>
       </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
       <c r="O17" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>233880</v>
+        <v>232235</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18">
         <v>1</v>
       </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
       <c r="O18" s="5">
         <f t="shared" si="0"/>
-        <v>0.29411764705882354</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>234009</v>
+        <v>233880</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="J19">
         <v>1</v>
       </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
       <c r="O19" s="5">
         <f t="shared" si="0"/>
-        <v>0.82352941176470584</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>234341</v>
+        <v>234009</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -4327,7 +5359,7 @@
         <v>1</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -4338,14 +5370,20 @@
       <c r="J20">
         <v>1</v>
       </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
       <c r="O20" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>234944</v>
+        <v>234341</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -4366,6 +5404,12 @@
         <v>1</v>
       </c>
       <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="M21">
         <v>1</v>
       </c>
       <c r="O21" s="5">
@@ -4375,7 +5419,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>235980</v>
+        <v>234944</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -4396,16 +5440,22 @@
         <v>1</v>
       </c>
       <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="M22">
         <v>0</v>
       </c>
       <c r="O22" s="5">
         <f t="shared" si="0"/>
-        <v>0.82352941176470584</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>236212</v>
+        <v>235980</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -4414,10 +5464,10 @@
         <v>1</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -4426,16 +5476,22 @@
         <v>1</v>
       </c>
       <c r="J23">
+        <v>0.75</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="M23">
         <v>0</v>
       </c>
       <c r="O23" s="5">
         <f t="shared" si="0"/>
-        <v>0.52941176470588236</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>239197</v>
+        <v>236212</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -4444,10 +5500,10 @@
         <v>1</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -4456,16 +5512,22 @@
         <v>1</v>
       </c>
       <c r="J24">
-        <v>1</v>
+        <v>0.75</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
       </c>
       <c r="O24" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>239272</v>
+        <v>239197</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -4486,6 +5548,12 @@
         <v>1</v>
       </c>
       <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="M25">
         <v>1</v>
       </c>
       <c r="O25" s="5">
@@ -4495,7 +5563,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>240231</v>
+        <v>239272</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -4518,14 +5586,20 @@
       <c r="J26">
         <v>1</v>
       </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
       <c r="O26" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>242056</v>
+        <v>240231</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -4548,14 +5622,20 @@
       <c r="J27">
         <v>1</v>
       </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
       <c r="O27" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>244277</v>
+        <v>242056</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -4578,74 +5658,128 @@
       <c r="J28">
         <v>1</v>
       </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
       <c r="O28" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>245146</v>
+        <v>244277</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
       </c>
       <c r="O29" s="5">
         <f t="shared" si="0"/>
-        <v>5.8823529411764705E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30">
+        <v>245146</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="O30" s="5">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31">
         <v>245365</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="H30">
-        <v>1</v>
-      </c>
-      <c r="J30">
-        <v>1</v>
-      </c>
-      <c r="O30" s="5">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="O31" s="5">
+        <f t="shared" si="0"/>
+        <v>0.84</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="O2:O30">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="O2:O31">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.5"/>
@@ -4665,7 +5799,7 @@
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4742,9 +5876,15 @@
       <c r="J2">
         <v>1</v>
       </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
       <c r="O2" s="5">
-        <f>(B2*1+C2*2+D2*2+E2*3+F2*3+H2*3+J2*3)/17</f>
-        <v>0.88235294117647056</v>
+        <f>(B2*1+C2*2+D2*2+E2*3+F2*3+H2*3+J2*3+K2*4+M2*4)/25</f>
+        <v>0.6</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -4772,9 +5912,15 @@
       <c r="J3">
         <v>0</v>
       </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O37" si="0">(B3*1+C3*2+D3*2+E3*3+F3*3+H3*3+J3*3)/17</f>
-        <v>5.8823529411764705E-2</v>
+        <f t="shared" ref="O3:O37" si="0">(B3*1+C3*2+D3*2+E3*3+F3*3+H3*3+J3*3+K3*4+M3*4)/25</f>
+        <v>0.04</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -4788,23 +5934,29 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
       <c r="O4" s="5">
         <f t="shared" si="0"/>
-        <v>0.17647058823529413</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -4818,7 +5970,7 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -4832,9 +5984,15 @@
       <c r="J5">
         <v>1</v>
       </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
       <c r="O5" s="5">
         <f t="shared" si="0"/>
-        <v>0.88235294117647056</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -4862,9 +6020,15 @@
       <c r="J6">
         <v>1</v>
       </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
       <c r="O6" s="5">
         <f t="shared" si="0"/>
-        <v>0.41176470588235292</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -4892,6 +6056,12 @@
       <c r="J7">
         <v>1</v>
       </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
       <c r="O7" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4922,6 +6092,12 @@
       <c r="J8">
         <v>1</v>
       </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
       <c r="O8" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4935,7 +6111,7 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -4944,7 +6120,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -4952,9 +6128,15 @@
       <c r="J9">
         <v>1</v>
       </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
       <c r="O9" s="5">
         <f t="shared" si="0"/>
-        <v>0.41176470588235292</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -4982,9 +6164,15 @@
       <c r="J10">
         <v>1</v>
       </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
       <c r="O10" s="5">
         <f t="shared" si="0"/>
-        <v>0.88235294117647056</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -5012,6 +6200,12 @@
       <c r="J11">
         <v>1</v>
       </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
       <c r="O11" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5042,9 +6236,15 @@
       <c r="J12">
         <v>1</v>
       </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
       <c r="O12" s="5">
         <f t="shared" si="0"/>
-        <v>0.88235294117647056</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -5072,9 +6272,15 @@
       <c r="J13">
         <v>0</v>
       </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
       <c r="O13" s="5">
         <f t="shared" si="0"/>
-        <v>0.17647058823529413</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -5102,9 +6308,15 @@
       <c r="J14">
         <v>1</v>
       </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
       <c r="O14" s="5">
         <f t="shared" si="0"/>
-        <v>0.88235294117647056</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -5132,9 +6344,15 @@
       <c r="J15">
         <v>1</v>
       </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
       <c r="O15" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -5162,9 +6380,15 @@
       <c r="J16">
         <v>0</v>
       </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
       <c r="O16" s="5">
         <f t="shared" si="0"/>
-        <v>0.17647058823529413</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -5192,9 +6416,15 @@
       <c r="J17">
         <v>0</v>
       </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
       <c r="O17" s="5">
         <f t="shared" si="0"/>
-        <v>0.70588235294117652</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -5222,6 +6452,12 @@
       <c r="J18">
         <v>1</v>
       </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
       <c r="O18" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5252,6 +6488,12 @@
       <c r="J19">
         <v>1</v>
       </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
       <c r="O19" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5282,9 +6524,15 @@
       <c r="J20">
         <v>1</v>
       </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
       <c r="O20" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -5312,6 +6560,12 @@
       <c r="J21">
         <v>1</v>
       </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
       <c r="O21" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5334,7 +6588,7 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -5342,9 +6596,15 @@
       <c r="J22">
         <v>0</v>
       </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
       <c r="O22" s="5">
         <f t="shared" si="0"/>
-        <v>0.6470588235294118</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -5372,9 +6632,15 @@
       <c r="J23">
         <v>1</v>
       </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
       <c r="O23" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -5402,9 +6668,15 @@
       <c r="J24">
         <v>0</v>
       </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
       <c r="O24" s="5">
         <f t="shared" si="0"/>
-        <v>5.8823529411764705E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -5432,6 +6704,12 @@
       <c r="J25">
         <v>1</v>
       </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
       <c r="O25" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5462,9 +6740,15 @@
       <c r="J26">
         <v>0</v>
       </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
       <c r="O26" s="5">
         <f t="shared" si="0"/>
-        <v>0.70588235294117652</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -5492,6 +6776,12 @@
       <c r="J27">
         <v>1</v>
       </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
       <c r="O27" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5517,14 +6807,20 @@
         <v>0</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J28">
         <v>1</v>
       </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
       <c r="O28" s="5">
         <f t="shared" si="0"/>
-        <v>0.35294117647058826</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -5552,9 +6848,15 @@
       <c r="J29">
         <v>0</v>
       </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
       <c r="O29" s="5">
         <f t="shared" si="0"/>
-        <v>5.8823529411764705E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -5565,10 +6867,10 @@
         <v>1</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -5582,9 +6884,15 @@
       <c r="J30">
         <v>1</v>
       </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
       <c r="O30" s="5">
         <f t="shared" si="0"/>
-        <v>0.58823529411764708</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -5601,7 +6909,7 @@
         <v>1</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -5612,9 +6920,15 @@
       <c r="J31">
         <v>1</v>
       </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
       <c r="O31" s="5">
         <f t="shared" si="0"/>
-        <v>0.82352941176470584</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
@@ -5631,20 +6945,26 @@
         <v>1</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="F32">
         <v>0</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J32">
         <v>0</v>
       </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
       <c r="O32" s="5">
         <f t="shared" si="0"/>
-        <v>0.29411764705882354</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
@@ -5672,9 +6992,15 @@
       <c r="J33">
         <v>1</v>
       </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
       <c r="O33" s="5">
         <f t="shared" si="0"/>
-        <v>0.82352941176470584</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
@@ -5702,6 +7028,12 @@
       <c r="J34">
         <v>1</v>
       </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
       <c r="O34" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5732,9 +7064,15 @@
       <c r="J35">
         <v>1</v>
       </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
       <c r="O35" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
@@ -5762,9 +7100,15 @@
       <c r="J36">
         <v>1</v>
       </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
       <c r="O36" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
@@ -5792,14 +7136,20 @@
       <c r="J37">
         <v>0</v>
       </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
       <c r="O37" s="5">
         <f t="shared" si="0"/>
-        <v>5.8823529411764705E-2</v>
+        <v>0.04</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="O2:O37">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.5"/>
@@ -5816,18 +7166,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -5900,14 +7250,14 @@
       <c r="J2" s="2">
         <v>3</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>23</v>
+      <c r="K2" s="2">
+        <v>4</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -5962,7 +7312,7 @@
       </c>
       <c r="D7">
         <f>COUNTA('Turma F'!A2:A50)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <f>COUNTA('Turma G'!A2:A50)</f>
@@ -5970,7 +7320,7 @@
       </c>
       <c r="F7">
         <f>SUM(B7:E7)</f>
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -5987,7 +7337,7 @@
       </c>
       <c r="D8" s="4">
         <f t="shared" si="0"/>
-        <v>0.87878787878787878</v>
+        <v>0.90909090909090906</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
@@ -5995,287 +7345,404 @@
       </c>
       <c r="F8" s="4">
         <f t="shared" si="0"/>
-        <v>0.85507246376811596</v>
+        <v>0.8623188405797102</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="4">
         <f>SUM('Turma D'!O2:O50)/B6</f>
-        <v>0.49197860962566842</v>
+        <v>0.50606060606060588</v>
       </c>
       <c r="C9" s="4">
         <f>SUM('Turma E'!O2:O50)/C6</f>
-        <v>0.56356736242884242</v>
+        <v>0.54774193548387096</v>
       </c>
       <c r="D9" s="4">
         <f>SUM('Turma F'!O2:O50)/D6</f>
-        <v>0.62566844919786102</v>
+        <v>0.61121212121212132</v>
       </c>
       <c r="E9" s="4">
         <f>SUM('Turma G'!O2:O50)/E6</f>
-        <v>0.60832137733142033</v>
+        <v>0.60073170731707293</v>
       </c>
       <c r="F9" s="4">
         <f>AVERAGE(B9:E9)</f>
-        <v>0.57238394964594808</v>
+        <v>0.56643659251841783</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="4">
         <f>SUM('Turma D'!O2:O50)/B7</f>
-        <v>0.57983193277310918</v>
+        <v>0.59642857142857131</v>
       </c>
       <c r="C10" s="4">
         <f>SUM('Turma E'!O2:O50)/C7</f>
-        <v>0.69882352941176462</v>
+        <v>0.67920000000000003</v>
       </c>
       <c r="D10" s="4">
         <f>SUM('Turma F'!O2:O50)/D7</f>
-        <v>0.71196754563894527</v>
+        <v>0.67233333333333334</v>
       </c>
       <c r="E10" s="4">
         <f>SUM('Turma G'!O2:O50)/E7</f>
-        <v>0.69281045751633985</v>
+        <v>0.68416666666666648</v>
       </c>
       <c r="F10" s="4">
         <f>AVERAGE(B10:E10)</f>
-        <v>0.67085836633503981</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+        <v>0.65803214285714284</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B11">
+        <f>COUNTIF('Turma D'!O2:O29,"&gt; 0.5")</f>
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <f>COUNTIF('Turma E'!O2:O50,"&gt; 0.5")</f>
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <f>COUNTIF('Turma F'!O2:O50,"&gt; 0.5")</f>
+        <v>23</v>
+      </c>
+      <c r="E11">
+        <f>COUNTIF('Turma G'!O2:O50,"&gt; 0.5")</f>
+        <v>29</v>
+      </c>
+      <c r="F11">
+        <f>SUM(B11:E11)</f>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="4">
+        <f>(B11/B6)</f>
+        <v>0.63636363636363635</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" ref="C12:F12" si="1">(C11/C6)</f>
+        <v>0.67741935483870963</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="1"/>
+        <v>0.69696969696969702</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="1"/>
+        <v>0.70731707317073167</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" si="1"/>
+        <v>0.6811594202898551</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="4">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4">
         <f>SUM('Turma D'!B2:B50)/B6</f>
-        <v>0.78787878787878785</v>
-      </c>
-      <c r="C14" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C16" s="4">
         <f>SUM('Turma E'!B3:B50)/C6</f>
-        <v>0.77419354838709675</v>
-      </c>
-      <c r="D14" s="4">
+        <v>0.79838709677419351</v>
+      </c>
+      <c r="D16" s="4">
         <f>SUM('Turma F'!B2:B50)/D6</f>
-        <v>0.81818181818181823</v>
-      </c>
-      <c r="E14" s="4">
+        <v>0.88636363636363635</v>
+      </c>
+      <c r="E16" s="4">
         <f>SUM('Turma G'!B2:B50)/E6</f>
         <v>0.87804878048780488</v>
       </c>
-      <c r="F14" s="4">
-        <f>AVERAGE(B14:E14)</f>
-        <v>0.81457573373387693</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="4">
-        <f>SUM('Turma D'!C2:C50)/B6</f>
-        <v>0.63636363636363635</v>
-      </c>
-      <c r="C15" s="4">
-        <f>SUM('Turma E'!C3:C50)/C6</f>
-        <v>0.58064516129032262</v>
-      </c>
-      <c r="D15" s="4">
-        <f>SUM('Turma F'!C2:C50)/D6</f>
-        <v>0.72727272727272729</v>
-      </c>
-      <c r="E15" s="4">
-        <f>SUM('Turma G'!C2:C50)/E6</f>
-        <v>0.68292682926829273</v>
-      </c>
-      <c r="F15" s="4">
-        <f>AVERAGE(B15:E15)</f>
-        <v>0.65680208854874478</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="4">
-        <f>SUM('Turma D'!D2:D50)/B6</f>
-        <v>0.42424242424242425</v>
-      </c>
-      <c r="C16" s="4">
-        <f>SUM('Turma E'!D3:D50)/C6</f>
-        <v>0.4838709677419355</v>
-      </c>
-      <c r="D16" s="4">
-        <f>SUM('Turma F'!D2:D50)/D6</f>
-        <v>0.63636363636363635</v>
-      </c>
-      <c r="E16" s="4">
-        <f>SUM('Turma G'!D2:D50)/E6</f>
-        <v>0.46341463414634149</v>
-      </c>
       <c r="F16" s="4">
         <f>AVERAGE(B16:E16)</f>
-        <v>0.50197291562358437</v>
+        <v>0.849033211739742</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B17" s="4">
-        <f>SUM('Turma D'!E2:E50)/B6</f>
-        <v>0.45454545454545453</v>
+        <f>SUM('Turma D'!C2:C50)/B6</f>
+        <v>0.68181818181818177</v>
       </c>
       <c r="C17" s="4">
-        <f>SUM('Turma E'!E3:E50)/C6</f>
-        <v>0.41935483870967744</v>
+        <f>SUM('Turma E'!C3:C50)/C6</f>
+        <v>0.62903225806451613</v>
       </c>
       <c r="D17" s="4">
-        <f>SUM('Turma F'!E2:E50)/D6</f>
-        <v>0.5757575757575758</v>
+        <f>SUM('Turma F'!C2:C50)/D6</f>
+        <v>0.79545454545454541</v>
       </c>
       <c r="E17" s="4">
-        <f>SUM('Turma G'!E2:E50)/E6</f>
-        <v>0.53658536585365857</v>
+        <f>SUM('Turma G'!C2:C50)/E6</f>
+        <v>0.71951219512195119</v>
       </c>
       <c r="F17" s="4">
         <f>AVERAGE(B17:E17)</f>
-        <v>0.49656080871659158</v>
+        <v>0.70645429511479874</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B18" s="4">
-        <f>SUM('Turma D'!F2:F50)/B6</f>
-        <v>0.42424242424242425</v>
+        <f>SUM('Turma D'!D2:D50)/B6</f>
+        <v>0.46969696969696972</v>
       </c>
       <c r="C18" s="4">
-        <f>SUM('Turma E'!F3:F50)/C6</f>
-        <v>0.54838709677419351</v>
+        <f>SUM('Turma E'!D3:D50)/C6</f>
+        <v>0.55645161290322576</v>
       </c>
       <c r="D18" s="4">
-        <f>SUM('Turma F'!F2:F50)/D6</f>
-        <v>0.60606060606060608</v>
+        <f>SUM('Turma F'!D2:D50)/D6</f>
+        <v>0.70454545454545459</v>
       </c>
       <c r="E18" s="4">
-        <f>SUM('Turma G'!F2:F50)/E6</f>
-        <v>0.58536585365853655</v>
+        <f>SUM('Turma G'!D2:D50)/E6</f>
+        <v>0.51829268292682928</v>
       </c>
       <c r="F18" s="4">
         <f>AVERAGE(B18:E18)</f>
-        <v>0.54101399518394011</v>
+        <v>0.56224668001811984</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="B19" s="4">
+        <f>SUM('Turma D'!E2:E50)/B6</f>
+        <v>0.47727272727272729</v>
+      </c>
+      <c r="C19" s="4">
+        <f>SUM('Turma E'!E3:E50)/C6</f>
+        <v>0.49193548387096775</v>
+      </c>
+      <c r="D19" s="4">
+        <f>SUM('Turma F'!E2:E50)/D6</f>
+        <v>0.64393939393939392</v>
+      </c>
+      <c r="E19" s="4">
+        <f>SUM('Turma G'!E2:E50)/E6</f>
+        <v>0.59146341463414631</v>
+      </c>
+      <c r="F19" s="4">
+        <f>AVERAGE(B19:E19)</f>
+        <v>0.55115275492930882</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" s="4">
-        <f>SUM('Turma D'!H2:H50)/B6</f>
-        <v>0.51515151515151514</v>
+        <f>SUM('Turma D'!F2:F50)/B6</f>
+        <v>0.53787878787878785</v>
       </c>
       <c r="C20" s="4">
-        <f>SUM('Turma E'!H2:H50)/B6</f>
-        <v>0.5757575757575758</v>
+        <f>SUM('Turma E'!F3:F50)/C6</f>
+        <v>0.59677419354838712</v>
       </c>
       <c r="D20" s="4">
-        <f>SUM('Turma F'!H2:H50)/B6</f>
-        <v>0.60606060606060608</v>
+        <f>SUM('Turma F'!F2:F50)/D6</f>
+        <v>0.69696969696969702</v>
       </c>
       <c r="E20" s="4">
-        <f>SUM('Turma G'!H2:H50)/B6</f>
-        <v>0.81818181818181823</v>
+        <f>SUM('Turma G'!F2:F50)/E6</f>
+        <v>0.6402439024390244</v>
       </c>
       <c r="F20" s="4">
-        <f t="shared" ref="F20:F22" si="1">AVERAGE(B20:E20)</f>
-        <v>0.62878787878787878</v>
+        <f>AVERAGE(B20:E20)</f>
+        <v>0.61796664520897415</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+        <v>16</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B22" s="4">
-        <f>SUM('Turma D'!J2:J50)/B6</f>
-        <v>0.42424242424242425</v>
+        <f>SUM('Turma D'!H2:H50)/B6</f>
+        <v>0.62878787878787878</v>
       </c>
       <c r="C22" s="4">
-        <f>SUM('Turma E'!J2:J50)/B6</f>
-        <v>0.60606060606060608</v>
+        <f>SUM('Turma E'!H2:H50)/C6</f>
+        <v>0.70967741935483875</v>
       </c>
       <c r="D22" s="4">
-        <f>SUM('Turma F'!J2:J50)/B6</f>
-        <v>0.5757575757575758</v>
+        <f>SUM('Turma F'!H2:H50)/D6</f>
+        <v>0.69696969696969702</v>
       </c>
       <c r="E22" s="4">
-        <f>SUM('Turma G'!J2:J50)/B6</f>
-        <v>0.75757575757575757</v>
+        <f>SUM('Turma G'!H2:H50)/E6</f>
+        <v>0.71341463414634143</v>
       </c>
       <c r="F22" s="4">
-        <f t="shared" si="1"/>
-        <v>0.59090909090909083</v>
+        <f>AVERAGE(B22:E22)</f>
+        <v>0.68721240731468891</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="B24" s="4">
+        <f>SUM('Turma D'!J2:J50)/B6</f>
+        <v>0.53787878787878785</v>
+      </c>
+      <c r="C24" s="4">
+        <f>SUM('Turma E'!J2:J50)/C6</f>
+        <v>0.69354838709677424</v>
+      </c>
+      <c r="D24" s="4">
+        <f>SUM('Turma F'!J2:J50)/D6</f>
+        <v>0.68939393939393945</v>
+      </c>
+      <c r="E24" s="4">
+        <f>SUM('Turma G'!J2:J50)/E6</f>
+        <v>0.6097560975609756</v>
+      </c>
+      <c r="F24" s="4">
+        <f>AVERAGE(B24:E24)</f>
+        <v>0.63264430298261931</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="4">
+        <f>SUM('Turma D'!H2:H50)/B6</f>
+        <v>0.62878787878787878</v>
+      </c>
+      <c r="C25" s="4">
+        <f>SUM('Turma E'!H2:H50)/C6</f>
+        <v>0.70967741935483875</v>
+      </c>
+      <c r="D25" s="4">
+        <f>SUM('Turma F'!H2:H50)/D6</f>
+        <v>0.69696969696969702</v>
+      </c>
+      <c r="E25" s="4">
+        <f>SUM('Turma G'!H2:H50)/E6</f>
+        <v>0.71341463414634143</v>
+      </c>
+      <c r="F25" s="4">
+        <f>AVERAGE(B25:E25)</f>
+        <v>0.68721240731468891</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
+      <c r="B27" s="4">
+        <f>SUM('Turma D'!M2:M50)/B6</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="C27" s="4">
+        <f>SUM('Turma E'!M2:M50)/C6</f>
+        <v>6.4516129032258063E-2</v>
+      </c>
+      <c r="D27" s="4">
+        <f>SUM('Turma F'!M2:M50)/D6</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="E27" s="4">
+        <f>SUM('Turma G'!M2:M50)/E6</f>
+        <v>0.34146341463414637</v>
+      </c>
+      <c r="F27" s="4">
+        <f>AVERAGE(B27:E27)</f>
+        <v>0.19240397682569202</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="12"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="7"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="12"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>